<commit_message>
Few Scenarios implemented for "Add Education Details"
</commit_message>
<xml_diff>
--- a/Manual Testcases/MarsCompetitionTask.xlsx
+++ b/Manual Testcases/MarsCompetitionTask.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVP Studio-Intern\Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVP Studio-Intern\Automation\MVPStudio.CompetitionTask\Manual Testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBD76953-1B82-4631-9F8F-1A9EC2CD6297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70970430-9A8F-4874-A686-7755D3F1F91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{76365835-A07E-489C-AD48-A72AEBBB6E84}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="563">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -2685,7 +2685,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2701,6 +2701,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA3DBFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC189F7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2782,7 +2794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2869,6 +2881,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2887,11 +2905,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3209,8 +3227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7098D8-86C2-4136-8563-CCDC432BDD79}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3358,7 +3376,7 @@
       <c r="B6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="40" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -3382,7 +3400,9 @@
       <c r="J6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="9"/>
+      <c r="K6" s="17" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
@@ -3398,13 +3418,13 @@
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="41" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -3431,9 +3451,9 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A9" s="38"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="4" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="41" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -3460,9 +3480,9 @@
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A10" s="38"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="4" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="41" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -3489,9 +3509,9 @@
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A11" s="38"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="4" t="s">
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="41" t="s">
         <v>50</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -3518,9 +3538,9 @@
       <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A12" s="38"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="4" t="s">
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="40" t="s">
         <v>55</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -3547,8 +3567,8 @@
       <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="38"/>
-      <c r="B13" s="39"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -3560,9 +3580,9 @@
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A14" s="38"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="4" t="s">
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="41" t="s">
         <v>59</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -3589,9 +3609,9 @@
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="4" t="s">
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="41" t="s">
         <v>64</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -3618,9 +3638,9 @@
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="38"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="4" t="s">
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="41" t="s">
         <v>69</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -3647,9 +3667,9 @@
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="38"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="4" t="s">
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="41" t="s">
         <v>74</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -3676,9 +3696,9 @@
       <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A18" s="38"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="4" t="s">
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="40" t="s">
         <v>80</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -3718,13 +3738,13 @@
       <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="40" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -3751,9 +3771,9 @@
       <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="38"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="4" t="s">
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="40" t="s">
         <v>91</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -3780,9 +3800,9 @@
       <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="38"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="4" t="s">
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="40" t="s">
         <v>95</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -3809,9 +3829,9 @@
       <c r="K22" s="9"/>
     </row>
     <row r="23" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A23" s="38"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="4" t="s">
+      <c r="A23" s="32"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="40" t="s">
         <v>98</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -3838,9 +3858,9 @@
       <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A24" s="38"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="4" t="s">
+      <c r="A24" s="32"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="40" t="s">
         <v>101</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -3880,10 +3900,10 @@
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="33" t="s">
         <v>105</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -3913,8 +3933,8 @@
       <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A27" s="38"/>
-      <c r="B27" s="39"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="4" t="s">
         <v>109</v>
       </c>
@@ -3942,8 +3962,8 @@
       <c r="K27" s="9"/>
     </row>
     <row r="28" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="38"/>
-      <c r="B28" s="39"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="4" t="s">
         <v>114</v>
       </c>
@@ -3971,8 +3991,8 @@
       <c r="K28" s="9"/>
     </row>
     <row r="29" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A29" s="38"/>
-      <c r="B29" s="39"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="33"/>
       <c r="C29" s="4" t="s">
         <v>119</v>
       </c>
@@ -4000,8 +4020,8 @@
       <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A30" s="38"/>
-      <c r="B30" s="39"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="4" t="s">
         <v>124</v>
       </c>
@@ -4048,7 +4068,7 @@
       <c r="B32" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="40" t="s">
         <v>130</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -4092,7 +4112,7 @@
       <c r="B34" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="40" t="s">
         <v>136</v>
       </c>
       <c r="D34" s="5" t="s">
@@ -4182,7 +4202,7 @@
       <c r="B38" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="40" t="s">
         <v>150</v>
       </c>
       <c r="D38" s="4" t="s">
@@ -4314,10 +4334,10 @@
       <c r="K43" s="9"/>
     </row>
     <row r="44" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="37" t="s">
         <v>171</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -4347,8 +4367,8 @@
       <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A45" s="33"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="38"/>
       <c r="C45" s="4" t="s">
         <v>177</v>
       </c>
@@ -4376,8 +4396,8 @@
       <c r="K45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A46" s="33"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="38"/>
       <c r="C46" s="4" t="s">
         <v>180</v>
       </c>
@@ -4405,8 +4425,8 @@
       <c r="K46" s="9"/>
     </row>
     <row r="47" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A47" s="33"/>
-      <c r="B47" s="36"/>
+      <c r="A47" s="35"/>
+      <c r="B47" s="38"/>
       <c r="C47" s="4" t="s">
         <v>183</v>
       </c>
@@ -4434,8 +4454,8 @@
       <c r="K47" s="9"/>
     </row>
     <row r="48" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A48" s="33"/>
-      <c r="B48" s="36"/>
+      <c r="A48" s="35"/>
+      <c r="B48" s="38"/>
       <c r="C48" s="4" t="s">
         <v>187</v>
       </c>
@@ -4463,8 +4483,8 @@
       <c r="K48" s="9"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" s="33"/>
-      <c r="B49" s="36"/>
+      <c r="A49" s="35"/>
+      <c r="B49" s="38"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -4476,8 +4496,8 @@
       <c r="K49" s="9"/>
     </row>
     <row r="50" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="33"/>
-      <c r="B50" s="36"/>
+      <c r="A50" s="35"/>
+      <c r="B50" s="38"/>
       <c r="C50" s="4" t="s">
         <v>190</v>
       </c>
@@ -4505,8 +4525,8 @@
       <c r="K50" s="9"/>
     </row>
     <row r="51" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="33"/>
-      <c r="B51" s="36"/>
+      <c r="A51" s="35"/>
+      <c r="B51" s="38"/>
       <c r="C51" s="4" t="s">
         <v>193</v>
       </c>
@@ -4534,8 +4554,8 @@
       <c r="K51" s="9"/>
     </row>
     <row r="52" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="33"/>
-      <c r="B52" s="36"/>
+      <c r="A52" s="35"/>
+      <c r="B52" s="38"/>
       <c r="C52" s="4" t="s">
         <v>196</v>
       </c>
@@ -4563,8 +4583,8 @@
       <c r="K52" s="9"/>
     </row>
     <row r="53" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="33"/>
-      <c r="B53" s="36"/>
+      <c r="A53" s="35"/>
+      <c r="B53" s="38"/>
       <c r="C53" s="4" t="s">
         <v>199</v>
       </c>
@@ -4592,8 +4612,8 @@
       <c r="K53" s="9"/>
     </row>
     <row r="54" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="34"/>
-      <c r="B54" s="37"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="39"/>
       <c r="C54" s="4" t="s">
         <v>203</v>
       </c>
@@ -4634,10 +4654,10 @@
       <c r="K55" s="9"/>
     </row>
     <row r="56" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="32" t="s">
+      <c r="A56" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="B56" s="35" t="s">
+      <c r="B56" s="37" t="s">
         <v>206</v>
       </c>
       <c r="C56" s="4" t="s">
@@ -4667,8 +4687,8 @@
       <c r="K56" s="9"/>
     </row>
     <row r="57" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="33"/>
-      <c r="B57" s="36"/>
+      <c r="A57" s="35"/>
+      <c r="B57" s="38"/>
       <c r="C57" s="4" t="s">
         <v>210</v>
       </c>
@@ -4696,8 +4716,8 @@
       <c r="K57" s="9"/>
     </row>
     <row r="58" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="33"/>
-      <c r="B58" s="36"/>
+      <c r="A58" s="35"/>
+      <c r="B58" s="38"/>
       <c r="C58" s="4" t="s">
         <v>213</v>
       </c>
@@ -4725,8 +4745,8 @@
       <c r="K58" s="9"/>
     </row>
     <row r="59" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A59" s="33"/>
-      <c r="B59" s="36"/>
+      <c r="A59" s="35"/>
+      <c r="B59" s="38"/>
       <c r="C59" s="4" t="s">
         <v>215</v>
       </c>
@@ -4754,8 +4774,8 @@
       <c r="K59" s="9"/>
     </row>
     <row r="60" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A60" s="34"/>
-      <c r="B60" s="37"/>
+      <c r="A60" s="36"/>
+      <c r="B60" s="39"/>
       <c r="C60" s="4" t="s">
         <v>218</v>
       </c>
@@ -4783,7 +4803,7 @@
       <c r="K60" s="9"/>
     </row>
     <row r="61" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="32" t="s">
+      <c r="A61" s="34" t="s">
         <v>221</v>
       </c>
       <c r="B61" s="25"/>
@@ -4798,8 +4818,8 @@
       <c r="K61" s="9"/>
     </row>
     <row r="62" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="33"/>
-      <c r="B62" s="35" t="s">
+      <c r="A62" s="35"/>
+      <c r="B62" s="37" t="s">
         <v>222</v>
       </c>
       <c r="C62" s="4" t="s">
@@ -4829,8 +4849,8 @@
       <c r="K62" s="9"/>
     </row>
     <row r="63" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A63" s="33"/>
-      <c r="B63" s="36"/>
+      <c r="A63" s="35"/>
+      <c r="B63" s="38"/>
       <c r="C63" s="4" t="s">
         <v>227</v>
       </c>
@@ -4858,8 +4878,8 @@
       <c r="K63" s="9"/>
     </row>
     <row r="64" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="33"/>
-      <c r="B64" s="36"/>
+      <c r="A64" s="35"/>
+      <c r="B64" s="38"/>
       <c r="C64" s="4" t="s">
         <v>232</v>
       </c>
@@ -4887,8 +4907,8 @@
       <c r="K64" s="9"/>
     </row>
     <row r="65" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="33"/>
-      <c r="B65" s="36"/>
+      <c r="A65" s="35"/>
+      <c r="B65" s="38"/>
       <c r="C65" s="4" t="s">
         <v>235</v>
       </c>
@@ -4916,8 +4936,8 @@
       <c r="K65" s="9"/>
     </row>
     <row r="66" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A66" s="34"/>
-      <c r="B66" s="37"/>
+      <c r="A66" s="36"/>
+      <c r="B66" s="39"/>
       <c r="C66" s="4" t="s">
         <v>239</v>
       </c>
@@ -5050,10 +5070,10 @@
       <c r="K71" s="9"/>
     </row>
     <row r="72" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A72" s="32" t="s">
+      <c r="A72" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="B72" s="32" t="s">
+      <c r="B72" s="34" t="s">
         <v>258</v>
       </c>
       <c r="C72" s="4" t="s">
@@ -5081,8 +5101,8 @@
       <c r="K72" s="17"/>
     </row>
     <row r="73" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="33"/>
-      <c r="B73" s="33"/>
+      <c r="A73" s="35"/>
+      <c r="B73" s="35"/>
       <c r="C73" s="4" t="s">
         <v>264</v>
       </c>
@@ -5108,8 +5128,8 @@
       <c r="K73" s="17"/>
     </row>
     <row r="74" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="34"/>
-      <c r="B74" s="34"/>
+      <c r="A74" s="36"/>
+      <c r="B74" s="36"/>
       <c r="C74" s="4" t="s">
         <v>269</v>
       </c>
@@ -5148,10 +5168,10 @@
       <c r="K75" s="17"/>
     </row>
     <row r="76" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A76" s="32" t="s">
+      <c r="A76" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="B76" s="35" t="s">
+      <c r="B76" s="37" t="s">
         <v>274</v>
       </c>
       <c r="C76" s="18" t="s">
@@ -5181,8 +5201,8 @@
       <c r="K76" s="24"/>
     </row>
     <row r="77" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A77" s="34"/>
-      <c r="B77" s="37"/>
+      <c r="A77" s="36"/>
+      <c r="B77" s="39"/>
       <c r="C77" s="18" t="s">
         <v>280</v>
       </c>
@@ -5269,10 +5289,10 @@
       <c r="K80" s="24"/>
     </row>
     <row r="81" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A81" s="32" t="s">
+      <c r="A81" s="34" t="s">
         <v>353</v>
       </c>
-      <c r="B81" s="35" t="s">
+      <c r="B81" s="37" t="s">
         <v>291</v>
       </c>
       <c r="C81" s="4" t="s">
@@ -5302,8 +5322,8 @@
       <c r="K81" s="24"/>
     </row>
     <row r="82" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A82" s="33"/>
-      <c r="B82" s="36"/>
+      <c r="A82" s="35"/>
+      <c r="B82" s="38"/>
       <c r="C82" s="4" t="s">
         <v>295</v>
       </c>
@@ -5331,8 +5351,8 @@
       <c r="K82" s="9"/>
     </row>
     <row r="83" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A83" s="34"/>
-      <c r="B83" s="37"/>
+      <c r="A83" s="36"/>
+      <c r="B83" s="39"/>
       <c r="C83" s="4" t="s">
         <v>300</v>
       </c>
@@ -5371,10 +5391,10 @@
       <c r="K84" s="9"/>
     </row>
     <row r="85" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A85" s="32" t="s">
+      <c r="A85" s="34" t="s">
         <v>354</v>
       </c>
-      <c r="B85" s="35" t="s">
+      <c r="B85" s="37" t="s">
         <v>305</v>
       </c>
       <c r="C85" s="4" t="s">
@@ -5404,8 +5424,8 @@
       <c r="K85" s="9"/>
     </row>
     <row r="86" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A86" s="33"/>
-      <c r="B86" s="36"/>
+      <c r="A86" s="35"/>
+      <c r="B86" s="38"/>
       <c r="C86" s="4" t="s">
         <v>308</v>
       </c>
@@ -5433,8 +5453,8 @@
       <c r="K86" s="9"/>
     </row>
     <row r="87" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A87" s="34"/>
-      <c r="B87" s="37"/>
+      <c r="A87" s="36"/>
+      <c r="B87" s="39"/>
       <c r="C87" s="4" t="s">
         <v>310</v>
       </c>
@@ -5520,17 +5540,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A44:A54"/>
-    <mergeCell ref="B44:B54"/>
-    <mergeCell ref="A56:A60"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A85:A87"/>
     <mergeCell ref="B85:B87"/>
     <mergeCell ref="B62:B66"/>
@@ -5540,6 +5549,17 @@
     <mergeCell ref="B76:B77"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="B81:B83"/>
+    <mergeCell ref="A44:A54"/>
+    <mergeCell ref="B44:B54"/>
+    <mergeCell ref="A56:A60"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="A61:A66"/>
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5738,10 +5758,10 @@
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="33" t="s">
         <v>364</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -5771,8 +5791,8 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="38"/>
-      <c r="B9" s="39"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="4" t="s">
         <v>42</v>
       </c>
@@ -5800,8 +5820,8 @@
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="38"/>
-      <c r="B10" s="39"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="4" t="s">
         <v>47</v>
       </c>
@@ -5829,8 +5849,8 @@
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="38"/>
-      <c r="B11" s="39"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="4" t="s">
         <v>50</v>
       </c>
@@ -5858,8 +5878,8 @@
       <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="38"/>
-      <c r="B12" s="39"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="4" t="s">
         <v>55</v>
       </c>
@@ -5887,8 +5907,8 @@
       <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="38"/>
-      <c r="B13" s="39"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -5900,8 +5920,8 @@
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="38"/>
-      <c r="B14" s="39"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="4" t="s">
         <v>59</v>
       </c>
@@ -5929,8 +5949,8 @@
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="4" t="s">
         <v>64</v>
       </c>
@@ -5958,8 +5978,8 @@
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="38"/>
-      <c r="B16" s="39"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="4" t="s">
         <v>69</v>
       </c>
@@ -5987,8 +6007,8 @@
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="38"/>
-      <c r="B17" s="39"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="4" t="s">
         <v>74</v>
       </c>
@@ -6016,8 +6036,8 @@
       <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="38"/>
-      <c r="B18" s="39"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="4" t="s">
         <v>80</v>
       </c>
@@ -6058,10 +6078,10 @@
       <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="33" t="s">
         <v>366</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -6089,8 +6109,8 @@
       <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="38"/>
-      <c r="B21" s="39"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="4" t="s">
         <v>91</v>
       </c>
@@ -6118,8 +6138,8 @@
       <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="38"/>
-      <c r="B22" s="39"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="4" t="s">
         <v>95</v>
       </c>
@@ -6160,10 +6180,10 @@
       <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="33" t="s">
         <v>368</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -6193,8 +6213,8 @@
       <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="38"/>
-      <c r="B25" s="39"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="4" t="s">
         <v>101</v>
       </c>
@@ -6222,8 +6242,8 @@
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="38"/>
-      <c r="B26" s="39"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="4" t="s">
         <v>106</v>
       </c>
@@ -6310,10 +6330,10 @@
       <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="37" t="s">
         <v>370</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -6343,8 +6363,8 @@
       <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A31" s="34"/>
-      <c r="B31" s="37"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="39"/>
       <c r="C31" s="4" t="s">
         <v>119</v>
       </c>
@@ -6523,10 +6543,10 @@
       <c r="K38" s="9"/>
     </row>
     <row r="39" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="38" t="s">
+      <c r="A39" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="33" t="s">
         <v>502</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -6556,8 +6576,8 @@
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="38"/>
-      <c r="B40" s="39"/>
+      <c r="A40" s="32"/>
+      <c r="B40" s="33"/>
       <c r="C40" s="4" t="s">
         <v>150</v>
       </c>
@@ -6585,8 +6605,8 @@
       <c r="K40" s="9"/>
     </row>
     <row r="41" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="38"/>
-      <c r="B41" s="39"/>
+      <c r="A41" s="32"/>
+      <c r="B41" s="33"/>
       <c r="C41" s="4" t="s">
         <v>157</v>
       </c>
@@ -6614,8 +6634,8 @@
       <c r="K41" s="9"/>
     </row>
     <row r="42" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="38"/>
-      <c r="B42" s="39"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="33"/>
       <c r="C42" s="4" t="s">
         <v>163</v>
       </c>
@@ -6643,8 +6663,8 @@
       <c r="K42" s="9"/>
     </row>
     <row r="43" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="38"/>
-      <c r="B43" s="39"/>
+      <c r="A43" s="32"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="4" t="s">
         <v>172</v>
       </c>
@@ -6672,8 +6692,8 @@
       <c r="K43" s="9"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="38"/>
-      <c r="B44" s="39"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -6685,8 +6705,8 @@
       <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="38"/>
-      <c r="B45" s="39"/>
+      <c r="A45" s="32"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="4" t="s">
         <v>177</v>
       </c>
@@ -6714,8 +6734,8 @@
       <c r="K45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="38"/>
-      <c r="B46" s="39"/>
+      <c r="A46" s="32"/>
+      <c r="B46" s="33"/>
       <c r="C46" s="4" t="s">
         <v>180</v>
       </c>
@@ -6743,8 +6763,8 @@
       <c r="K46" s="9"/>
     </row>
     <row r="47" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="38"/>
-      <c r="B47" s="39"/>
+      <c r="A47" s="32"/>
+      <c r="B47" s="33"/>
       <c r="C47" s="4" t="s">
         <v>183</v>
       </c>
@@ -6772,8 +6792,8 @@
       <c r="K47" s="9"/>
     </row>
     <row r="48" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="38"/>
-      <c r="B48" s="39"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="33"/>
       <c r="C48" s="4" t="s">
         <v>187</v>
       </c>
@@ -6801,8 +6821,8 @@
       <c r="K48" s="9"/>
     </row>
     <row r="49" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="38"/>
-      <c r="B49" s="39"/>
+      <c r="A49" s="32"/>
+      <c r="B49" s="33"/>
       <c r="C49" s="4" t="s">
         <v>190</v>
       </c>
@@ -6843,10 +6863,10 @@
       <c r="K50" s="9"/>
     </row>
     <row r="51" spans="1:1105" ht="87" x14ac:dyDescent="0.35">
-      <c r="A51" s="38" t="s">
+      <c r="A51" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="B51" s="39" t="s">
+      <c r="B51" s="33" t="s">
         <v>372</v>
       </c>
       <c r="C51" s="4" t="s">
@@ -6874,8 +6894,8 @@
       <c r="K51" s="9"/>
     </row>
     <row r="52" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="38"/>
-      <c r="B52" s="39"/>
+      <c r="A52" s="32"/>
+      <c r="B52" s="33"/>
       <c r="C52" s="4" t="s">
         <v>196</v>
       </c>
@@ -6903,8 +6923,8 @@
       <c r="K52" s="9"/>
     </row>
     <row r="53" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="38"/>
-      <c r="B53" s="39"/>
+      <c r="A53" s="32"/>
+      <c r="B53" s="33"/>
       <c r="C53" s="4" t="s">
         <v>199</v>
       </c>
@@ -6991,10 +7011,10 @@
       <c r="K56" s="9"/>
     </row>
     <row r="57" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="32" t="s">
+      <c r="A57" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="37" t="s">
         <v>526</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -7024,8 +7044,8 @@
       <c r="K57" s="11"/>
     </row>
     <row r="58" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="33"/>
-      <c r="B58" s="36"/>
+      <c r="A58" s="35"/>
+      <c r="B58" s="38"/>
       <c r="C58" s="4" t="s">
         <v>210</v>
       </c>
@@ -7053,8 +7073,8 @@
       <c r="K58" s="11"/>
     </row>
     <row r="59" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="34"/>
-      <c r="B59" s="37"/>
+      <c r="A59" s="36"/>
+      <c r="B59" s="39"/>
       <c r="C59" s="4" t="s">
         <v>213</v>
       </c>
@@ -12657,10 +12677,10 @@
       <c r="APM64" s="31"/>
     </row>
     <row r="65" spans="1:1105" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="38" t="s">
+      <c r="A65" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="B65" s="38" t="s">
+      <c r="B65" s="32" t="s">
         <v>374</v>
       </c>
       <c r="C65" s="4" t="s">
@@ -13782,8 +13802,8 @@
       <c r="APM65" s="31"/>
     </row>
     <row r="66" spans="1:1105" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="38"/>
-      <c r="B66" s="38"/>
+      <c r="A66" s="32"/>
+      <c r="B66" s="32"/>
       <c r="C66" s="4" t="s">
         <v>227</v>
       </c>
@@ -14903,8 +14923,8 @@
       <c r="APM66" s="31"/>
     </row>
     <row r="67" spans="1:1105" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="38"/>
-      <c r="B67" s="38"/>
+      <c r="A67" s="32"/>
+      <c r="B67" s="32"/>
       <c r="C67" s="4" t="s">
         <v>232</v>
       </c>
@@ -17131,10 +17151,10 @@
       <c r="APM68" s="31"/>
     </row>
     <row r="69" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="38" t="s">
+      <c r="A69" s="32" t="s">
         <v>273</v>
       </c>
-      <c r="B69" s="39" t="s">
+      <c r="B69" s="33" t="s">
         <v>415</v>
       </c>
       <c r="C69" s="4" t="s">
@@ -18258,8 +18278,8 @@
       <c r="APM69" s="31"/>
     </row>
     <row r="70" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="38"/>
-      <c r="B70" s="39"/>
+      <c r="A70" s="32"/>
+      <c r="B70" s="33"/>
       <c r="C70" s="4" t="s">
         <v>239</v>
       </c>
@@ -18346,10 +18366,10 @@
       <c r="K73" s="9"/>
     </row>
     <row r="74" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="38" t="s">
+      <c r="A74" s="32" t="s">
         <v>353</v>
       </c>
-      <c r="B74" s="39" t="s">
+      <c r="B74" s="33" t="s">
         <v>416</v>
       </c>
       <c r="C74" s="4" t="s">
@@ -18379,8 +18399,8 @@
       <c r="K74" s="9"/>
     </row>
     <row r="75" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="38"/>
-      <c r="B75" s="39"/>
+      <c r="A75" s="32"/>
+      <c r="B75" s="33"/>
       <c r="C75" s="4" t="s">
         <v>259</v>
       </c>
@@ -18408,8 +18428,8 @@
       <c r="K75" s="9"/>
     </row>
     <row r="76" spans="1:1105" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="38"/>
-      <c r="B76" s="39"/>
+      <c r="A76" s="32"/>
+      <c r="B76" s="33"/>
       <c r="C76" s="4" t="s">
         <v>264</v>
       </c>
@@ -18448,10 +18468,10 @@
       <c r="K77" s="9"/>
     </row>
     <row r="78" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A78" s="38" t="s">
+      <c r="A78" s="32" t="s">
         <v>354</v>
       </c>
-      <c r="B78" s="39" t="s">
+      <c r="B78" s="33" t="s">
         <v>417</v>
       </c>
       <c r="C78" s="4" t="s">
@@ -18481,8 +18501,8 @@
       <c r="K78" s="9"/>
     </row>
     <row r="79" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A79" s="38"/>
-      <c r="B79" s="39"/>
+      <c r="A79" s="32"/>
+      <c r="B79" s="33"/>
       <c r="C79" s="4" t="s">
         <v>275</v>
       </c>
@@ -18510,8 +18530,8 @@
       <c r="K79" s="9"/>
     </row>
     <row r="80" spans="1:1105" ht="58" x14ac:dyDescent="0.35">
-      <c r="A80" s="38"/>
-      <c r="B80" s="39"/>
+      <c r="A80" s="32"/>
+      <c r="B80" s="33"/>
       <c r="C80" s="4" t="s">
         <v>280</v>
       </c>
@@ -18551,12 +18571,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
     <mergeCell ref="A78:A80"/>
     <mergeCell ref="B78:B80"/>
     <mergeCell ref="B30:B31"/>
@@ -18573,6 +18587,12 @@
     <mergeCell ref="B39:B49"/>
     <mergeCell ref="A51:A53"/>
     <mergeCell ref="B51:B53"/>
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update for Education Feature implemented
</commit_message>
<xml_diff>
--- a/Manual Testcases/MarsCompetitionTask.xlsx
+++ b/Manual Testcases/MarsCompetitionTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVP Studio-Intern\Automation\MVPStudio.CompetitionTask\Manual Testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70970430-9A8F-4874-A686-7755D3F1F91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F63FFB-EEFD-4E95-A0EB-04A0D195DBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{76365835-A07E-489C-AD48-A72AEBBB6E84}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="564">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -551,52 +551,6 @@
 6. Select the year using "Year of graduation"
 drop-down
 7. Click the "Add" button </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Step 1: College/University Name: Anna University
-Country of College/University: India
-Title: B.Tech
-Degree: Bachelor of Engineering
-Year of graduation: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2015</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Step 2: College/University Name: Anna University
-Country of College/University: India
-Title: B.A
-Degree: Bachelor of Arts
-Year of graduation: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2015</t>
-    </r>
   </si>
   <si>
     <t>User is able to add multiple degrees in
@@ -2651,6 +2605,56 @@
     <t>1. Click the "Delete" icon for a particular education in one window
 2. Try to delete the different education details again in another browser.</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Step 1: College/University Name: Anna University
+Country of College/University: India
+Title: B.Tech
+Degree: Bachelor of Engineering
+Year of graduation: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2015</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Step 2: College/University Name: Annamalai University
+Country of College/University: India
+Title: B.A
+Degree: Bachelor of Arts
+Year of graduation: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2015</t>
+    </r>
+  </si>
+  <si>
+    <t>User is not able to add the education details. Get
+error message: "undefined"</t>
+  </si>
 </sst>
 </file>
 
@@ -2685,7 +2689,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2707,12 +2711,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC189F7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2794,7 +2792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2881,6 +2879,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2908,8 +2909,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3227,8 +3228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7098D8-86C2-4136-8563-CCDC432BDD79}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76:B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3288,7 +3289,7 @@
       <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="32" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -3332,7 +3333,7 @@
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="32" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -3376,7 +3377,7 @@
       <c r="B6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="32" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -3395,7 +3396,7 @@
         <v>33</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>19</v>
@@ -3418,13 +3419,13 @@
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="32" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -3440,10 +3441,10 @@
         <v>40</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>41</v>
@@ -3451,9 +3452,9 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="41" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="32" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -3472,7 +3473,7 @@
         <v>46</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>41</v>
@@ -3480,9 +3481,9 @@
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="41" t="s">
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="32" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -3492,16 +3493,16 @@
         <v>30</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>49</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>41</v>
@@ -3509,9 +3510,9 @@
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="41" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="32" t="s">
         <v>50</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -3527,7 +3528,7 @@
         <v>53</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>54</v>
@@ -3538,9 +3539,9 @@
       <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="40" t="s">
+      <c r="A12" s="33"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="32" t="s">
         <v>55</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -3556,10 +3557,10 @@
         <v>58</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>41</v>
@@ -3567,8 +3568,8 @@
       <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -3580,9 +3581,9 @@
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="41" t="s">
+      <c r="A14" s="33"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="32" t="s">
         <v>59</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -3601,7 +3602,7 @@
         <v>63</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>41</v>
@@ -3609,9 +3610,9 @@
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="41" t="s">
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="32" t="s">
         <v>64</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -3630,7 +3631,7 @@
         <v>68</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>41</v>
@@ -3638,9 +3639,9 @@
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="41" t="s">
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="32" t="s">
         <v>69</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -3659,7 +3660,7 @@
         <v>73</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>41</v>
@@ -3667,9 +3668,9 @@
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="32"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="41" t="s">
+      <c r="A17" s="33"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="32" t="s">
         <v>74</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -3696,9 +3697,9 @@
       <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="40" t="s">
+      <c r="A18" s="33"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="32" t="s">
         <v>80</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -3711,13 +3712,13 @@
         <v>82</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>84</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>41</v>
@@ -3738,17 +3739,17 @@
       <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="32" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>30</v>
@@ -3763,7 +3764,7 @@
         <v>90</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>19</v>
@@ -3771,9 +3772,9 @@
       <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="40" t="s">
+      <c r="A21" s="41"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="32" t="s">
         <v>91</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -3792,7 +3793,7 @@
         <v>90</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>19</v>
@@ -3800,13 +3801,13 @@
       <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="32"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="40" t="s">
+      <c r="A22" s="41"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="32" t="s">
         <v>95</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>30</v>
@@ -3821,7 +3822,7 @@
         <v>90</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>19</v>
@@ -3829,13 +3830,13 @@
       <c r="K22" s="9"/>
     </row>
     <row r="23" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A23" s="32"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="40" t="s">
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="32" t="s">
         <v>98</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>30</v>
@@ -3850,7 +3851,7 @@
         <v>90</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>19</v>
@@ -3858,13 +3859,13 @@
       <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A24" s="32"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="40" t="s">
+      <c r="A24" s="41"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="32" t="s">
         <v>101</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>30</v>
@@ -3879,7 +3880,7 @@
         <v>90</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>19</v>
@@ -3900,20 +3901,20 @@
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="32" t="s">
         <v>106</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>107</v>
@@ -3933,13 +3934,13 @@
       <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A27" s="32"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="4" t="s">
+      <c r="A27" s="33"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="32" t="s">
         <v>109</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>30</v>
@@ -3948,27 +3949,27 @@
         <v>110</v>
       </c>
       <c r="G27" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="H27" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="I27" s="5" t="s">
+      <c r="J27" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="K27" s="9"/>
     </row>
     <row r="28" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="32"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="4" t="s">
+      <c r="A28" s="33"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>30</v>
@@ -3977,13 +3978,13 @@
         <v>107</v>
       </c>
       <c r="G28" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="I28" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>41</v>
@@ -3991,13 +3992,13 @@
       <c r="K28" s="9"/>
     </row>
     <row r="29" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A29" s="32"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="4" t="s">
+      <c r="A29" s="33"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>30</v>
@@ -4006,13 +4007,13 @@
         <v>110</v>
       </c>
       <c r="G29" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>41</v>
@@ -4020,28 +4021,28 @@
       <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A30" s="32"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="4" t="s">
+      <c r="A30" s="33"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>328</v>
+        <v>563</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>19</v>
@@ -4063,16 +4064,16 @@
     </row>
     <row r="32" spans="1:11" ht="145" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="D32" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>131</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>30</v>
@@ -4082,13 +4083,13 @@
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I32" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="J32" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="K32" s="9"/>
     </row>
@@ -4107,16 +4108,16 @@
     </row>
     <row r="34" spans="1:11" ht="145" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>329</v>
-      </c>
-      <c r="C34" s="40" t="s">
+      <c r="D34" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>30</v>
@@ -4125,16 +4126,16 @@
         <v>110</v>
       </c>
       <c r="G34" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="I34" s="4" t="s">
-        <v>140</v>
-      </c>
       <c r="J34" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K34" s="9"/>
     </row>
@@ -4153,32 +4154,32 @@
     </row>
     <row r="36" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="D36" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="I36" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="J36" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K36" s="9"/>
     </row>
@@ -4197,31 +4198,31 @@
     </row>
     <row r="38" spans="1:11" ht="145" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="D38" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G38" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H38" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="I38" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>19</v>
@@ -4243,16 +4244,16 @@
     </row>
     <row r="40" spans="1:11" ht="145" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>30</v>
@@ -4264,10 +4265,10 @@
         <v>32</v>
       </c>
       <c r="H40" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I40" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>19</v>
@@ -4289,31 +4290,31 @@
     </row>
     <row r="42" spans="1:11" ht="145" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="C42" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="E42" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="F42" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="G42" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="H42" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H42" s="5" t="s">
-        <v>168</v>
-      </c>
       <c r="I42" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>19</v>
@@ -4334,32 +4335,32 @@
       <c r="K43" s="9"/>
     </row>
     <row r="44" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B44" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="C44" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="D44" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="F44" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>40</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>41</v>
@@ -4367,28 +4368,28 @@
       <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A45" s="35"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="4" t="s">
+      <c r="A45" s="36"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="E45" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F45" s="14" t="s">
         <v>178</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>179</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>45</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>41</v>
@@ -4396,28 +4397,28 @@
       <c r="K45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A46" s="35"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="4" t="s">
+      <c r="A46" s="36"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="E46" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F46" s="14" t="s">
         <v>181</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>182</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>49</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>41</v>
@@ -4425,28 +4426,28 @@
       <c r="K46" s="9"/>
     </row>
     <row r="47" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A47" s="35"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="4" t="s">
+      <c r="A47" s="36"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="E47" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F47" s="14" t="s">
         <v>184</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F47" s="14" t="s">
-        <v>185</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>53</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>19</v>
@@ -4454,28 +4455,28 @@
       <c r="K47" s="9"/>
     </row>
     <row r="48" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A48" s="35"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="4" t="s">
+      <c r="A48" s="36"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="E48" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F48" s="14" t="s">
         <v>188</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>189</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>58</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>41</v>
@@ -4483,8 +4484,8 @@
       <c r="K48" s="9"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" s="35"/>
-      <c r="B49" s="38"/>
+      <c r="A49" s="36"/>
+      <c r="B49" s="39"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -4496,28 +4497,28 @@
       <c r="K49" s="9"/>
     </row>
     <row r="50" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="35"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="4" t="s">
+      <c r="A50" s="36"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="E50" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F50" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>192</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>62</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>41</v>
@@ -4525,28 +4526,28 @@
       <c r="K50" s="9"/>
     </row>
     <row r="51" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="35"/>
-      <c r="B51" s="38"/>
-      <c r="C51" s="4" t="s">
+      <c r="A51" s="36"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="E51" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F51" s="10" t="s">
         <v>194</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>195</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>67</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>41</v>
@@ -4554,28 +4555,28 @@
       <c r="K51" s="9"/>
     </row>
     <row r="52" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="35"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="4" t="s">
+      <c r="A52" s="36"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="E52" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F52" s="10" t="s">
         <v>197</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>198</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>72</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>41</v>
@@ -4583,28 +4584,28 @@
       <c r="K52" s="9"/>
     </row>
     <row r="53" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="35"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="4" t="s">
+      <c r="A53" s="36"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="E53" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F53" s="10" t="s">
         <v>200</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>201</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>77</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>19</v>
@@ -4612,28 +4613,28 @@
       <c r="K53" s="9"/>
     </row>
     <row r="54" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="36"/>
-      <c r="B54" s="39"/>
-      <c r="C54" s="4" t="s">
-        <v>203</v>
+      <c r="A54" s="37"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="32" t="s">
+        <v>202</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>83</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>41</v>
@@ -4654,32 +4655,32 @@
       <c r="K55" s="9"/>
     </row>
     <row r="56" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="34" t="s">
+      <c r="A56" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="B56" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="B56" s="37" t="s">
+      <c r="C56" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="D56" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="E56" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F56" s="14" t="s">
         <v>208</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>209</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>89</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>19</v>
@@ -4687,28 +4688,28 @@
       <c r="K56" s="9"/>
     </row>
     <row r="57" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="35"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="4" t="s">
+      <c r="A57" s="36"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="E57" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F57" s="14" t="s">
         <v>211</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F57" s="14" t="s">
-        <v>212</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>94</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>19</v>
@@ -4716,28 +4717,28 @@
       <c r="K57" s="9"/>
     </row>
     <row r="58" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="35"/>
-      <c r="B58" s="38"/>
-      <c r="C58" s="4" t="s">
+      <c r="A58" s="36"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F58" s="14" t="s">
         <v>213</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F58" s="14" t="s">
-        <v>214</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>97</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>19</v>
@@ -4745,28 +4746,28 @@
       <c r="K58" s="9"/>
     </row>
     <row r="59" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A59" s="35"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="4" t="s">
+      <c r="A59" s="36"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="E59" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F59" s="14" t="s">
         <v>216</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>217</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>100</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>19</v>
@@ -4774,28 +4775,28 @@
       <c r="K59" s="9"/>
     </row>
     <row r="60" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A60" s="36"/>
-      <c r="B60" s="39"/>
-      <c r="C60" s="4" t="s">
+      <c r="A60" s="37"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D60" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="E60" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F60" s="14" t="s">
         <v>219</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>220</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>103</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J60" s="4" t="s">
         <v>19</v>
@@ -4803,8 +4804,8 @@
       <c r="K60" s="9"/>
     </row>
     <row r="61" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="34" t="s">
-        <v>221</v>
+      <c r="A61" s="35" t="s">
+        <v>220</v>
       </c>
       <c r="B61" s="25"/>
       <c r="C61" s="11"/>
@@ -4818,24 +4819,24 @@
       <c r="K61" s="9"/>
     </row>
     <row r="62" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="35"/>
-      <c r="B62" s="37" t="s">
+      <c r="A62" s="36"/>
+      <c r="B62" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="C62" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="D62" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="E62" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F62" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="E62" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F62" s="10" t="s">
+      <c r="G62" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>226</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>90</v>
@@ -4849,57 +4850,57 @@
       <c r="K62" s="9"/>
     </row>
     <row r="63" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A63" s="35"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="4" t="s">
+      <c r="A63" s="36"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="D63" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="E63" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="G63" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="E63" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="G63" s="5" t="s">
+      <c r="H63" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="I63" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="I63" s="5" t="s">
-        <v>231</v>
-      </c>
       <c r="J63" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K63" s="9"/>
     </row>
     <row r="64" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="35"/>
-      <c r="B64" s="38"/>
-      <c r="C64" s="4" t="s">
+      <c r="A64" s="36"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H64" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F64" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="H64" s="5" t="s">
+      <c r="I64" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>234</v>
       </c>
       <c r="J64" s="4" t="s">
         <v>41</v>
@@ -4907,28 +4908,28 @@
       <c r="K64" s="9"/>
     </row>
     <row r="65" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="35"/>
-      <c r="B65" s="38"/>
-      <c r="C65" s="4" t="s">
+      <c r="A65" s="36"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="E65" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H65" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="E65" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="H65" s="5" t="s">
+      <c r="I65" s="5" t="s">
         <v>237</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>238</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>41</v>
@@ -4936,28 +4937,28 @@
       <c r="K65" s="9"/>
     </row>
     <row r="66" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A66" s="36"/>
-      <c r="B66" s="39"/>
-      <c r="C66" s="4" t="s">
+      <c r="A66" s="37"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="E66" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F66" s="10" t="s">
         <v>240</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F66" s="10" t="s">
-        <v>241</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>19</v>
@@ -4979,31 +4980,31 @@
     </row>
     <row r="68" spans="1:11" ht="145" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="D68" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="E68" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>544</v>
+      </c>
+      <c r="G68" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="E68" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F68" s="14" t="s">
-        <v>545</v>
-      </c>
-      <c r="G68" s="4" t="s">
+      <c r="H68" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="H68" s="4" t="s">
+      <c r="I68" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="I68" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>19</v>
@@ -5025,31 +5026,31 @@
     </row>
     <row r="70" spans="1:11" ht="145" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="C70" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="D70" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="E70" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F70" s="10" t="s">
         <v>253</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F70" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H70" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="I70" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="I70" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>19</v>
@@ -5070,30 +5071,30 @@
       <c r="K71" s="9"/>
     </row>
     <row r="72" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A72" s="34" t="s">
+      <c r="A72" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="B72" s="35" t="s">
         <v>257</v>
       </c>
-      <c r="B72" s="34" t="s">
+      <c r="C72" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="D72" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="E72" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F72" s="21" t="s">
         <v>260</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F72" s="21" t="s">
-        <v>261</v>
       </c>
       <c r="G72" s="4"/>
       <c r="H72" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="I72" s="4" t="s">
         <v>262</v>
-      </c>
-      <c r="I72" s="4" t="s">
-        <v>263</v>
       </c>
       <c r="J72" s="22" t="s">
         <v>19</v>
@@ -5101,26 +5102,26 @@
       <c r="K72" s="17"/>
     </row>
     <row r="73" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="35"/>
-      <c r="B73" s="35"/>
+      <c r="A73" s="36"/>
+      <c r="B73" s="36"/>
       <c r="C73" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D73" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="E73" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F73" s="21" t="s">
         <v>265</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F73" s="21" t="s">
-        <v>266</v>
       </c>
       <c r="G73" s="4"/>
       <c r="H73" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="I73" s="4" t="s">
         <v>267</v>
-      </c>
-      <c r="I73" s="4" t="s">
-        <v>268</v>
       </c>
       <c r="J73" s="22" t="s">
         <v>19</v>
@@ -5128,26 +5129,26 @@
       <c r="K73" s="17"/>
     </row>
     <row r="74" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="36"/>
-      <c r="B74" s="36"/>
+      <c r="A74" s="37"/>
+      <c r="B74" s="37"/>
       <c r="C74" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D74" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="E74" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F74" s="21" t="s">
         <v>270</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F74" s="21" t="s">
-        <v>271</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J74" s="22" t="s">
         <v>19</v>
@@ -5168,32 +5169,32 @@
       <c r="K75" s="17"/>
     </row>
     <row r="76" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A76" s="34" t="s">
+      <c r="A76" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="B76" s="38" t="s">
         <v>273</v>
       </c>
-      <c r="B76" s="37" t="s">
+      <c r="C76" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="C76" s="18" t="s">
+      <c r="D76" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="E76" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="E76" s="16" t="s">
+      <c r="F76" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="F76" s="23" t="s">
+      <c r="G76" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="H76" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="G76" s="15" t="s">
+      <c r="I76" s="16" t="s">
         <v>343</v>
-      </c>
-      <c r="H76" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="I76" s="16" t="s">
-        <v>344</v>
       </c>
       <c r="J76" s="16" t="s">
         <v>41</v>
@@ -5201,28 +5202,28 @@
       <c r="K76" s="24"/>
     </row>
     <row r="77" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A77" s="36"/>
-      <c r="B77" s="39"/>
+      <c r="A77" s="37"/>
+      <c r="B77" s="40"/>
       <c r="C77" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="D77" s="18" t="s">
         <v>280</v>
       </c>
-      <c r="D77" s="18" t="s">
+      <c r="E77" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="F77" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="E77" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="F77" s="21" t="s">
+      <c r="G77" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="H77" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="G77" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>283</v>
-      </c>
       <c r="I77" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>41</v>
@@ -5244,31 +5245,31 @@
     </row>
     <row r="79" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B79" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="D79" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="E79" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="E79" s="4" t="s">
+      <c r="F79" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="F79" s="21" t="s">
+      <c r="G79" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="H79" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="G79" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="H79" s="5" t="s">
+      <c r="I79" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="I79" s="5" t="s">
-        <v>290</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>19</v>
@@ -5289,32 +5290,32 @@
       <c r="K80" s="24"/>
     </row>
     <row r="81" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A81" s="34" t="s">
-        <v>353</v>
-      </c>
-      <c r="B81" s="37" t="s">
+      <c r="A81" s="35" t="s">
+        <v>352</v>
+      </c>
+      <c r="B81" s="38" t="s">
+        <v>290</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="C81" s="4" t="s">
-        <v>292</v>
-      </c>
       <c r="D81" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J81" s="4" t="s">
         <v>19</v>
@@ -5322,28 +5323,28 @@
       <c r="K81" s="24"/>
     </row>
     <row r="82" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A82" s="35"/>
-      <c r="B82" s="38"/>
+      <c r="A82" s="36"/>
+      <c r="B82" s="39"/>
       <c r="C82" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="E82" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="F82" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="I82" s="5" t="s">
         <v>348</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="F82" s="14" t="s">
-        <v>297</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="H82" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="I82" s="5" t="s">
-        <v>349</v>
       </c>
       <c r="J82" s="4" t="s">
         <v>19</v>
@@ -5351,26 +5352,26 @@
       <c r="K82" s="9"/>
     </row>
     <row r="83" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A83" s="36"/>
-      <c r="B83" s="39"/>
+      <c r="A83" s="37"/>
+      <c r="B83" s="40"/>
       <c r="C83" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="E83" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="F83" s="21" t="s">
         <v>302</v>
-      </c>
-      <c r="F83" s="21" t="s">
-        <v>303</v>
       </c>
       <c r="G83" s="4"/>
       <c r="H83" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J83" s="22" t="s">
         <v>19</v>
@@ -5391,29 +5392,29 @@
       <c r="K84" s="9"/>
     </row>
     <row r="85" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A85" s="34" t="s">
-        <v>354</v>
-      </c>
-      <c r="B85" s="37" t="s">
+      <c r="A85" s="35" t="s">
+        <v>353</v>
+      </c>
+      <c r="B85" s="38" t="s">
+        <v>304</v>
+      </c>
+      <c r="C85" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="C85" s="4" t="s">
-        <v>306</v>
-      </c>
       <c r="D85" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>34</v>
@@ -5424,28 +5425,28 @@
       <c r="K85" s="9"/>
     </row>
     <row r="86" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A86" s="35"/>
-      <c r="B86" s="38"/>
+      <c r="A86" s="36"/>
+      <c r="B86" s="39"/>
       <c r="C86" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="F86" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="H86" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="D86" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="F86" s="14" t="s">
-        <v>297</v>
-      </c>
-      <c r="G86" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="H86" s="5" t="s">
-        <v>309</v>
-      </c>
       <c r="I86" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J86" s="4" t="s">
         <v>19</v>
@@ -5453,26 +5454,26 @@
       <c r="K86" s="9"/>
     </row>
     <row r="87" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A87" s="36"/>
-      <c r="B87" s="39"/>
+      <c r="A87" s="37"/>
+      <c r="B87" s="40"/>
       <c r="C87" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D87" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="E87" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="F87" s="21" t="s">
         <v>311</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="F87" s="21" t="s">
-        <v>312</v>
       </c>
       <c r="G87" s="4"/>
       <c r="H87" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="I87" s="5" t="s">
         <v>313</v>
-      </c>
-      <c r="I87" s="5" t="s">
-        <v>314</v>
       </c>
       <c r="J87" s="22" t="s">
         <v>19</v>
@@ -5494,31 +5495,31 @@
     </row>
     <row r="89" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A89" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="B89" s="27" t="s">
         <v>355</v>
       </c>
-      <c r="B89" s="27" t="s">
+      <c r="C89" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="D89" s="27" t="s">
         <v>357</v>
-      </c>
-      <c r="D89" s="27" t="s">
-        <v>358</v>
       </c>
       <c r="E89" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F89" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="G89" s="27" t="s">
         <v>359</v>
-      </c>
-      <c r="G89" s="27" t="s">
-        <v>360</v>
       </c>
       <c r="H89" s="17" t="s">
         <v>90</v>
       </c>
       <c r="I89" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J89" s="4" t="s">
         <v>41</v>
@@ -5628,26 +5629,26 @@
         <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>19</v>
@@ -5684,7 +5685,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
@@ -5716,28 +5717,28 @@
         <v>26</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>19</v>
@@ -5758,32 +5759,32 @@
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="33" t="s">
-        <v>364</v>
+      <c r="B8" s="34" t="s">
+        <v>363</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>41</v>
@@ -5791,28 +5792,28 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>41</v>
@@ -5820,28 +5821,28 @@
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>41</v>
@@ -5849,28 +5850,28 @@
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>41</v>
@@ -5878,28 +5879,28 @@
       <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>41</v>
@@ -5907,8 +5908,8 @@
       <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -5920,28 +5921,28 @@
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>41</v>
@@ -5949,28 +5950,28 @@
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>41</v>
@@ -5978,28 +5979,28 @@
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>41</v>
@@ -6007,28 +6008,28 @@
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="32"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>41</v>
@@ -6036,28 +6037,28 @@
       <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="4" t="s">
         <v>80</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>41</v>
@@ -6078,30 +6079,30 @@
       <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="33" t="s">
-        <v>366</v>
+      <c r="B20" s="34" t="s">
+        <v>365</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>445</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>446</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>19</v>
@@ -6109,28 +6110,28 @@
       <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="4" t="s">
         <v>91</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>473</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>474</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>421</v>
-      </c>
       <c r="H21" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>445</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>446</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>19</v>
@@ -6138,28 +6139,28 @@
       <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="32"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="4" t="s">
         <v>95</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H22" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>445</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>446</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>19</v>
@@ -6180,32 +6181,32 @@
       <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="B24" s="33" t="s">
-        <v>368</v>
+      <c r="B24" s="34" t="s">
+        <v>367</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>98</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>19</v>
@@ -6213,28 +6214,28 @@
       <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="32"/>
-      <c r="B25" s="33"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="4" t="s">
         <v>101</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G25" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>452</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>453</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>41</v>
@@ -6242,28 +6243,28 @@
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="32"/>
-      <c r="B26" s="33"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="34"/>
       <c r="C26" s="4" t="s">
         <v>106</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>19</v>
@@ -6285,34 +6286,34 @@
     </row>
     <row r="28" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G28" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>456</v>
       </c>
-      <c r="H28" s="4" t="s">
-        <v>457</v>
-      </c>
       <c r="I28" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K28" s="9"/>
     </row>
@@ -6330,32 +6331,32 @@
       <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A30" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>370</v>
+      <c r="A30" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>369</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G30" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="I30" s="4" t="s">
         <v>499</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>500</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>19</v>
@@ -6363,31 +6364,31 @@
       <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A31" s="36"/>
-      <c r="B31" s="39"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H31" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="I31" s="4" t="s">
-        <v>462</v>
-      </c>
       <c r="J31" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K31" s="9"/>
     </row>
@@ -6406,31 +6407,31 @@
     </row>
     <row r="33" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>501</v>
-      </c>
-      <c r="G33" s="4" t="s">
+      <c r="H33" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>19</v>
@@ -6452,31 +6453,31 @@
     </row>
     <row r="35" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E35" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="F35" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>460</v>
-      </c>
       <c r="I35" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>19</v>
@@ -6498,31 +6499,31 @@
     </row>
     <row r="37" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G37" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="I37" s="5" t="s">
         <v>486</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>487</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>19</v>
@@ -6543,32 +6544,32 @@
       <c r="K38" s="9"/>
     </row>
     <row r="39" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>502</v>
+      <c r="A39" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>501</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H39" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="I39" s="5" t="s">
         <v>492</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>493</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>41</v>
@@ -6576,28 +6577,28 @@
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="32"/>
-      <c r="B40" s="33"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="34"/>
       <c r="C40" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>41</v>
@@ -6605,28 +6606,28 @@
       <c r="K40" s="9"/>
     </row>
     <row r="41" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="32"/>
-      <c r="B41" s="33"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="34"/>
       <c r="C41" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>41</v>
@@ -6634,28 +6635,28 @@
       <c r="K41" s="9"/>
     </row>
     <row r="42" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="32"/>
-      <c r="B42" s="33"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>41</v>
@@ -6663,28 +6664,28 @@
       <c r="K42" s="9"/>
     </row>
     <row r="43" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="32"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G43" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="H43" s="4" t="s">
-        <v>492</v>
-      </c>
       <c r="I43" s="5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>41</v>
@@ -6692,8 +6693,8 @@
       <c r="K43" s="9"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="32"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -6705,28 +6706,28 @@
       <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="32"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G45" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="I45" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>41</v>
@@ -6734,28 +6735,28 @@
       <c r="K45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="32"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>41</v>
@@ -6763,28 +6764,28 @@
       <c r="K46" s="9"/>
     </row>
     <row r="47" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="32"/>
-      <c r="B47" s="33"/>
+      <c r="A47" s="33"/>
+      <c r="B47" s="34"/>
       <c r="C47" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>41</v>
@@ -6792,28 +6793,28 @@
       <c r="K47" s="9"/>
     </row>
     <row r="48" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="32"/>
-      <c r="B48" s="33"/>
+      <c r="A48" s="33"/>
+      <c r="B48" s="34"/>
       <c r="C48" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>41</v>
@@ -6821,28 +6822,28 @@
       <c r="K48" s="9"/>
     </row>
     <row r="49" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="32"/>
-      <c r="B49" s="33"/>
+      <c r="A49" s="33"/>
+      <c r="B49" s="34"/>
       <c r="C49" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F49" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G49" s="5" t="s">
-        <v>508</v>
-      </c>
       <c r="H49" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>41</v>
@@ -6863,30 +6864,30 @@
       <c r="K50" s="9"/>
     </row>
     <row r="51" spans="1:1105" ht="87" x14ac:dyDescent="0.35">
-      <c r="A51" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="B51" s="33" t="s">
-        <v>372</v>
+      <c r="A51" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>371</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="I51" s="5" t="s">
         <v>521</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>522</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>19</v>
@@ -6894,28 +6895,28 @@
       <c r="K51" s="9"/>
     </row>
     <row r="52" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="32"/>
-      <c r="B52" s="33"/>
+      <c r="A52" s="33"/>
+      <c r="B52" s="34"/>
       <c r="C52" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H52" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="I52" s="5" t="s">
         <v>521</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>522</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>19</v>
@@ -6923,28 +6924,28 @@
       <c r="K52" s="9"/>
     </row>
     <row r="53" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="32"/>
-      <c r="B53" s="33"/>
+      <c r="A53" s="33"/>
+      <c r="B53" s="34"/>
       <c r="C53" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H53" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="I53" s="5" t="s">
         <v>521</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>522</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>19</v>
@@ -6966,31 +6967,31 @@
     </row>
     <row r="55" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B55" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>525</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G55" s="5" t="s">
+      <c r="H55" s="5" t="s">
         <v>540</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="I55" s="4" t="s">
         <v>541</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>542</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>19</v>
@@ -7011,32 +7012,32 @@
       <c r="K56" s="9"/>
     </row>
     <row r="57" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="34" t="s">
+      <c r="A57" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="37" t="s">
-        <v>526</v>
+      <c r="B57" s="38" t="s">
+        <v>525</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>19</v>
@@ -7044,28 +7045,28 @@
       <c r="K57" s="11"/>
     </row>
     <row r="58" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="35"/>
-      <c r="B58" s="38"/>
+      <c r="A58" s="36"/>
+      <c r="B58" s="39"/>
       <c r="C58" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>41</v>
@@ -7073,28 +7074,28 @@
       <c r="K58" s="11"/>
     </row>
     <row r="59" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="36"/>
-      <c r="B59" s="39"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="40"/>
       <c r="C59" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F59" s="10" t="s">
+        <v>515</v>
+      </c>
+      <c r="G59" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="G59" s="5" t="s">
+      <c r="H59" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="I59" s="30" t="s">
         <v>518</v>
-      </c>
-      <c r="I59" s="30" t="s">
-        <v>519</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>19</v>
@@ -8210,31 +8211,31 @@
     </row>
     <row r="61" spans="1:1105" s="29" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>244</v>
-      </c>
       <c r="C61" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G61" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H61" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="I61" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>19</v>
@@ -10444,31 +10445,31 @@
     </row>
     <row r="63" spans="1:1105" s="29" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="B63" s="4" t="s">
-        <v>251</v>
-      </c>
       <c r="C63" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H63" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="I63" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="J63" s="4" t="s">
         <v>19</v>
@@ -12677,30 +12678,30 @@
       <c r="APM64" s="31"/>
     </row>
     <row r="65" spans="1:1105" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="32" t="s">
-        <v>257</v>
-      </c>
-      <c r="B65" s="32" t="s">
+      <c r="A65" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="B65" s="33" t="s">
+        <v>373</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>375</v>
-      </c>
       <c r="E65" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="F65" s="21" t="s">
         <v>531</v>
-      </c>
-      <c r="F65" s="21" t="s">
-        <v>532</v>
       </c>
       <c r="G65" s="4"/>
       <c r="H65" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="I65" s="4" t="s">
         <v>534</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>535</v>
       </c>
       <c r="J65" s="22" t="s">
         <v>19</v>
@@ -13802,26 +13803,26 @@
       <c r="APM65" s="31"/>
     </row>
     <row r="66" spans="1:1105" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="32"/>
-      <c r="B66" s="32"/>
+      <c r="A66" s="33"/>
+      <c r="B66" s="33"/>
       <c r="C66" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G66" s="4"/>
       <c r="H66" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="I66" s="4" t="s">
         <v>267</v>
-      </c>
-      <c r="I66" s="4" t="s">
-        <v>268</v>
       </c>
       <c r="J66" s="22" t="s">
         <v>19</v>
@@ -14923,26 +14924,26 @@
       <c r="APM66" s="31"/>
     </row>
     <row r="67" spans="1:1105" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="32"/>
-      <c r="B67" s="32"/>
+      <c r="A67" s="33"/>
+      <c r="B67" s="33"/>
       <c r="C67" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D67" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="F67" s="21" t="s">
         <v>270</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="F67" s="21" t="s">
-        <v>271</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J67" s="22" t="s">
         <v>19</v>
@@ -17151,32 +17152,32 @@
       <c r="APM68" s="31"/>
     </row>
     <row r="69" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="32" t="s">
-        <v>273</v>
-      </c>
-      <c r="B69" s="33" t="s">
-        <v>415</v>
+      <c r="A69" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="B69" s="34" t="s">
+        <v>414</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F69" s="23" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I69" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J69" s="16" t="s">
         <v>41</v>
@@ -18278,28 +18279,28 @@
       <c r="APM69" s="31"/>
     </row>
     <row r="70" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="32"/>
-      <c r="B70" s="33"/>
+      <c r="A70" s="33"/>
+      <c r="B70" s="34"/>
       <c r="C70" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F70" s="21" t="s">
+        <v>526</v>
+      </c>
+      <c r="G70" s="15" t="s">
+        <v>529</v>
+      </c>
+      <c r="H70" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="G70" s="15" t="s">
-        <v>530</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>528</v>
-      </c>
       <c r="I70" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>41</v>
@@ -18321,31 +18322,31 @@
     </row>
     <row r="72" spans="1:1105" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E72" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="F72" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="F72" s="21" t="s">
+      <c r="G72" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="H72" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="G72" s="5" t="s">
-        <v>514</v>
-      </c>
-      <c r="H72" s="5" t="s">
+      <c r="I72" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="I72" s="5" t="s">
-        <v>290</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>19</v>
@@ -18366,32 +18367,32 @@
       <c r="K73" s="9"/>
     </row>
     <row r="74" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="B74" s="33" t="s">
-        <v>416</v>
+      <c r="A74" s="33" t="s">
+        <v>352</v>
+      </c>
+      <c r="B74" s="34" t="s">
+        <v>415</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E74" s="17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F74" s="14" t="s">
+        <v>548</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="H74" s="5" t="s">
         <v>549</v>
       </c>
-      <c r="G74" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>550</v>
-      </c>
       <c r="I74" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>19</v>
@@ -18399,28 +18400,28 @@
       <c r="K74" s="9"/>
     </row>
     <row r="75" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="32"/>
-      <c r="B75" s="33"/>
+      <c r="A75" s="33"/>
+      <c r="B75" s="34"/>
       <c r="C75" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E75" s="27" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F75" s="14" t="s">
+        <v>550</v>
+      </c>
+      <c r="G75" s="5" t="s">
         <v>551</v>
       </c>
-      <c r="G75" s="5" t="s">
-        <v>552</v>
-      </c>
       <c r="H75" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>19</v>
@@ -18428,26 +18429,26 @@
       <c r="K75" s="9"/>
     </row>
     <row r="76" spans="1:1105" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="32"/>
-      <c r="B76" s="33"/>
+      <c r="A76" s="33"/>
+      <c r="B76" s="34"/>
       <c r="C76" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E76" s="27" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F76" s="21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G76" s="4"/>
       <c r="H76" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J76" s="22" t="s">
         <v>19</v>
@@ -18468,32 +18469,32 @@
       <c r="K77" s="9"/>
     </row>
     <row r="78" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A78" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="B78" s="33" t="s">
-        <v>417</v>
+      <c r="A78" s="33" t="s">
+        <v>353</v>
+      </c>
+      <c r="B78" s="34" t="s">
+        <v>416</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E78" s="17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F78" s="26" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G78" s="27" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H78" s="27" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I78" s="27" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="J78" s="17" t="s">
         <v>19</v>
@@ -18501,28 +18502,28 @@
       <c r="K78" s="9"/>
     </row>
     <row r="79" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A79" s="32"/>
-      <c r="B79" s="33"/>
+      <c r="A79" s="33"/>
+      <c r="B79" s="34"/>
       <c r="C79" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F79" s="26" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G79" s="27" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H79" s="27" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I79" s="27" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="J79" s="17" t="s">
         <v>19</v>
@@ -18530,26 +18531,26 @@
       <c r="K79" s="9"/>
     </row>
     <row r="80" spans="1:1105" ht="58" x14ac:dyDescent="0.35">
-      <c r="A80" s="32"/>
-      <c r="B80" s="33"/>
+      <c r="A80" s="33"/>
+      <c r="B80" s="34"/>
       <c r="C80" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F80" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G80" s="17"/>
       <c r="H80" s="27" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I80" s="27" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="J80" s="17" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Add Certification Details Initial Commit
</commit_message>
<xml_diff>
--- a/Manual Testcases/MarsCompetitionTask.xlsx
+++ b/Manual Testcases/MarsCompetitionTask.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVP Studio-Intern\Automation\MVPStudio.CompetitionTask\Manual Testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F63FFB-EEFD-4E95-A0EB-04A0D195DBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13842CEF-6216-4202-ACFA-D025135DD509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{76365835-A07E-489C-AD48-A72AEBBB6E84}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{76365835-A07E-489C-AD48-A72AEBBB6E84}"/>
   </bookViews>
   <sheets>
     <sheet name="Education" sheetId="1" r:id="rId1"/>
@@ -1953,11 +1953,6 @@
 "has been added to your certification"</t>
   </si>
   <si>
-    <t>User is able to add the certification details successfully
-and see the success message:
-"aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaahas been added to your certification"</t>
-  </si>
-  <si>
     <t>User shouldn't be able to add certifications with huge certificate 
 provider name</t>
   </si>
@@ -2654,6 +2649,11 @@
   <si>
     <t>User is not able to add the education details. Get
 error message: "undefined"</t>
+  </si>
+  <si>
+    <t>User is able to add the certification details successfully
+and see the success message:
+"aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa has been added to your certification"</t>
   </si>
 </sst>
 </file>
@@ -2792,7 +2792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2882,12 +2882,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2906,11 +2900,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3228,7 +3231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7098D8-86C2-4136-8563-CCDC432BDD79}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="B76" sqref="B76:B77"/>
     </sheetView>
   </sheetViews>
@@ -3419,10 +3422,10 @@
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="40" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="32" t="s">
@@ -3452,8 +3455,8 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A9" s="33"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="32" t="s">
         <v>42</v>
       </c>
@@ -3481,8 +3484,8 @@
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A10" s="33"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="32" t="s">
         <v>47</v>
       </c>
@@ -3510,8 +3513,8 @@
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="32" t="s">
         <v>50</v>
       </c>
@@ -3539,8 +3542,8 @@
       <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A12" s="33"/>
-      <c r="B12" s="34"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="32" t="s">
         <v>55</v>
       </c>
@@ -3568,8 +3571,8 @@
       <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="33"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -3581,8 +3584,8 @@
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A14" s="33"/>
-      <c r="B14" s="34"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="32" t="s">
         <v>59</v>
       </c>
@@ -3610,8 +3613,8 @@
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="32" t="s">
         <v>64</v>
       </c>
@@ -3639,8 +3642,8 @@
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="32" t="s">
         <v>69</v>
       </c>
@@ -3668,8 +3671,8 @@
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="32" t="s">
         <v>74</v>
       </c>
@@ -3697,8 +3700,8 @@
       <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="32" t="s">
         <v>80</v>
       </c>
@@ -3901,10 +3904,10 @@
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="40" t="s">
         <v>105</v>
       </c>
       <c r="C26" s="32" t="s">
@@ -3914,7 +3917,7 @@
         <v>323</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>107</v>
@@ -3934,8 +3937,8 @@
       <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A27" s="33"/>
-      <c r="B27" s="34"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="32" t="s">
         <v>109</v>
       </c>
@@ -3949,7 +3952,7 @@
         <v>110</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>325</v>
@@ -3963,8 +3966,8 @@
       <c r="K27" s="9"/>
     </row>
     <row r="28" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="33"/>
-      <c r="B28" s="34"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="32" t="s">
         <v>113</v>
       </c>
@@ -3992,8 +3995,8 @@
       <c r="K28" s="9"/>
     </row>
     <row r="29" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A29" s="33"/>
-      <c r="B29" s="34"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="32" t="s">
         <v>118</v>
       </c>
@@ -4021,8 +4024,8 @@
       <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A30" s="33"/>
-      <c r="B30" s="34"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="32" t="s">
         <v>123</v>
       </c>
@@ -4042,7 +4045,7 @@
         <v>126</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>19</v>
@@ -4335,10 +4338,10 @@
       <c r="K43" s="9"/>
     </row>
     <row r="44" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B44" s="38" t="s">
+      <c r="B44" s="36" t="s">
         <v>170</v>
       </c>
       <c r="C44" s="32" t="s">
@@ -4368,8 +4371,8 @@
       <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A45" s="36"/>
-      <c r="B45" s="39"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="37"/>
       <c r="C45" s="32" t="s">
         <v>176</v>
       </c>
@@ -4397,8 +4400,8 @@
       <c r="K45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A46" s="36"/>
-      <c r="B46" s="39"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="37"/>
       <c r="C46" s="32" t="s">
         <v>179</v>
       </c>
@@ -4426,8 +4429,8 @@
       <c r="K46" s="9"/>
     </row>
     <row r="47" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A47" s="36"/>
-      <c r="B47" s="39"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="37"/>
       <c r="C47" s="32" t="s">
         <v>182</v>
       </c>
@@ -4455,8 +4458,8 @@
       <c r="K47" s="9"/>
     </row>
     <row r="48" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A48" s="36"/>
-      <c r="B48" s="39"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="37"/>
       <c r="C48" s="32" t="s">
         <v>186</v>
       </c>
@@ -4484,8 +4487,8 @@
       <c r="K48" s="9"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" s="36"/>
-      <c r="B49" s="39"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="37"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -4497,8 +4500,8 @@
       <c r="K49" s="9"/>
     </row>
     <row r="50" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="36"/>
-      <c r="B50" s="39"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="37"/>
       <c r="C50" s="32" t="s">
         <v>189</v>
       </c>
@@ -4526,8 +4529,8 @@
       <c r="K50" s="9"/>
     </row>
     <row r="51" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="36"/>
-      <c r="B51" s="39"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="37"/>
       <c r="C51" s="32" t="s">
         <v>192</v>
       </c>
@@ -4555,8 +4558,8 @@
       <c r="K51" s="9"/>
     </row>
     <row r="52" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="36"/>
-      <c r="B52" s="39"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="37"/>
       <c r="C52" s="32" t="s">
         <v>195</v>
       </c>
@@ -4584,8 +4587,8 @@
       <c r="K52" s="9"/>
     </row>
     <row r="53" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="36"/>
-      <c r="B53" s="39"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="37"/>
       <c r="C53" s="32" t="s">
         <v>198</v>
       </c>
@@ -4613,8 +4616,8 @@
       <c r="K53" s="9"/>
     </row>
     <row r="54" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="37"/>
-      <c r="B54" s="40"/>
+      <c r="A54" s="35"/>
+      <c r="B54" s="38"/>
       <c r="C54" s="32" t="s">
         <v>202</v>
       </c>
@@ -4655,10 +4658,10 @@
       <c r="K55" s="9"/>
     </row>
     <row r="56" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="B56" s="38" t="s">
+      <c r="B56" s="36" t="s">
         <v>205</v>
       </c>
       <c r="C56" s="32" t="s">
@@ -4688,8 +4691,8 @@
       <c r="K56" s="9"/>
     </row>
     <row r="57" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="36"/>
-      <c r="B57" s="39"/>
+      <c r="A57" s="34"/>
+      <c r="B57" s="37"/>
       <c r="C57" s="32" t="s">
         <v>209</v>
       </c>
@@ -4717,8 +4720,8 @@
       <c r="K57" s="9"/>
     </row>
     <row r="58" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="36"/>
-      <c r="B58" s="39"/>
+      <c r="A58" s="34"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="32" t="s">
         <v>212</v>
       </c>
@@ -4746,8 +4749,8 @@
       <c r="K58" s="9"/>
     </row>
     <row r="59" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A59" s="36"/>
-      <c r="B59" s="39"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="37"/>
       <c r="C59" s="32" t="s">
         <v>214</v>
       </c>
@@ -4775,8 +4778,8 @@
       <c r="K59" s="9"/>
     </row>
     <row r="60" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A60" s="37"/>
-      <c r="B60" s="40"/>
+      <c r="A60" s="35"/>
+      <c r="B60" s="38"/>
       <c r="C60" s="32" t="s">
         <v>217</v>
       </c>
@@ -4804,7 +4807,7 @@
       <c r="K60" s="9"/>
     </row>
     <row r="61" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="33" t="s">
         <v>220</v>
       </c>
       <c r="B61" s="25"/>
@@ -4819,8 +4822,8 @@
       <c r="K61" s="9"/>
     </row>
     <row r="62" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="36"/>
-      <c r="B62" s="38" t="s">
+      <c r="A62" s="34"/>
+      <c r="B62" s="36" t="s">
         <v>221</v>
       </c>
       <c r="C62" s="32" t="s">
@@ -4850,8 +4853,8 @@
       <c r="K62" s="9"/>
     </row>
     <row r="63" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A63" s="36"/>
-      <c r="B63" s="39"/>
+      <c r="A63" s="34"/>
+      <c r="B63" s="37"/>
       <c r="C63" s="32" t="s">
         <v>226</v>
       </c>
@@ -4879,8 +4882,8 @@
       <c r="K63" s="9"/>
     </row>
     <row r="64" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="36"/>
-      <c r="B64" s="39"/>
+      <c r="A64" s="34"/>
+      <c r="B64" s="37"/>
       <c r="C64" s="32" t="s">
         <v>231</v>
       </c>
@@ -4908,8 +4911,8 @@
       <c r="K64" s="9"/>
     </row>
     <row r="65" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="36"/>
-      <c r="B65" s="39"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="37"/>
       <c r="C65" s="32" t="s">
         <v>234</v>
       </c>
@@ -4937,8 +4940,8 @@
       <c r="K65" s="9"/>
     </row>
     <row r="66" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A66" s="37"/>
-      <c r="B66" s="40"/>
+      <c r="A66" s="35"/>
+      <c r="B66" s="38"/>
       <c r="C66" s="32" t="s">
         <v>238</v>
       </c>
@@ -4995,7 +4998,7 @@
         <v>115</v>
       </c>
       <c r="F68" s="14" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>246</v>
@@ -5071,10 +5074,10 @@
       <c r="K71" s="9"/>
     </row>
     <row r="72" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A72" s="35" t="s">
+      <c r="A72" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="B72" s="35" t="s">
+      <c r="B72" s="33" t="s">
         <v>257</v>
       </c>
       <c r="C72" s="32" t="s">
@@ -5102,8 +5105,8 @@
       <c r="K72" s="17"/>
     </row>
     <row r="73" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="36"/>
-      <c r="B73" s="36"/>
+      <c r="A73" s="34"/>
+      <c r="B73" s="34"/>
       <c r="C73" s="4" t="s">
         <v>263</v>
       </c>
@@ -5129,8 +5132,8 @@
       <c r="K73" s="17"/>
     </row>
     <row r="74" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="37"/>
-      <c r="B74" s="37"/>
+      <c r="A74" s="35"/>
+      <c r="B74" s="35"/>
       <c r="C74" s="4" t="s">
         <v>268</v>
       </c>
@@ -5169,10 +5172,10 @@
       <c r="K75" s="17"/>
     </row>
     <row r="76" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A76" s="35" t="s">
+      <c r="A76" s="33" t="s">
         <v>272</v>
       </c>
-      <c r="B76" s="38" t="s">
+      <c r="B76" s="36" t="s">
         <v>273</v>
       </c>
       <c r="C76" s="18" t="s">
@@ -5202,8 +5205,8 @@
       <c r="K76" s="24"/>
     </row>
     <row r="77" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A77" s="37"/>
-      <c r="B77" s="40"/>
+      <c r="A77" s="35"/>
+      <c r="B77" s="38"/>
       <c r="C77" s="18" t="s">
         <v>279</v>
       </c>
@@ -5290,10 +5293,10 @@
       <c r="K80" s="24"/>
     </row>
     <row r="81" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A81" s="35" t="s">
+      <c r="A81" s="33" t="s">
         <v>352</v>
       </c>
-      <c r="B81" s="38" t="s">
+      <c r="B81" s="36" t="s">
         <v>290</v>
       </c>
       <c r="C81" s="4" t="s">
@@ -5323,8 +5326,8 @@
       <c r="K81" s="24"/>
     </row>
     <row r="82" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A82" s="36"/>
-      <c r="B82" s="39"/>
+      <c r="A82" s="34"/>
+      <c r="B82" s="37"/>
       <c r="C82" s="4" t="s">
         <v>294</v>
       </c>
@@ -5352,8 +5355,8 @@
       <c r="K82" s="9"/>
     </row>
     <row r="83" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A83" s="37"/>
-      <c r="B83" s="40"/>
+      <c r="A83" s="35"/>
+      <c r="B83" s="38"/>
       <c r="C83" s="4" t="s">
         <v>299</v>
       </c>
@@ -5392,10 +5395,10 @@
       <c r="K84" s="9"/>
     </row>
     <row r="85" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A85" s="35" t="s">
+      <c r="A85" s="33" t="s">
         <v>353</v>
       </c>
-      <c r="B85" s="38" t="s">
+      <c r="B85" s="36" t="s">
         <v>304</v>
       </c>
       <c r="C85" s="4" t="s">
@@ -5425,8 +5428,8 @@
       <c r="K85" s="9"/>
     </row>
     <row r="86" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A86" s="36"/>
-      <c r="B86" s="39"/>
+      <c r="A86" s="34"/>
+      <c r="B86" s="37"/>
       <c r="C86" s="4" t="s">
         <v>307</v>
       </c>
@@ -5454,8 +5457,8 @@
       <c r="K86" s="9"/>
     </row>
     <row r="87" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A87" s="37"/>
-      <c r="B87" s="40"/>
+      <c r="A87" s="35"/>
+      <c r="B87" s="38"/>
       <c r="C87" s="4" t="s">
         <v>309</v>
       </c>
@@ -5541,6 +5544,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A44:A54"/>
+    <mergeCell ref="B44:B54"/>
+    <mergeCell ref="A56:A60"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A85:A87"/>
     <mergeCell ref="B85:B87"/>
     <mergeCell ref="B62:B66"/>
@@ -5550,17 +5564,6 @@
     <mergeCell ref="B76:B77"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="B81:B83"/>
-    <mergeCell ref="A44:A54"/>
-    <mergeCell ref="B44:B54"/>
-    <mergeCell ref="A56:A60"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5570,8 +5573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DD1934-0003-4B65-8812-56E0F2750A75}">
   <dimension ref="A1:APM81"/>
   <sheetViews>
-    <sheetView topLeftCell="F67" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5629,9 +5632,9 @@
         <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>536</v>
-      </c>
-      <c r="C2" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -5648,7 +5651,7 @@
         <v>418</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>19</v>
@@ -5658,7 +5661,7 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="10"/>
@@ -5675,7 +5678,7 @@
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="32" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -5702,7 +5705,7 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="6"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="8"/>
@@ -5719,7 +5722,7 @@
       <c r="B6" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="32" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -5729,7 +5732,7 @@
         <v>419</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>421</v>
@@ -5759,13 +5762,13 @@
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="40" t="s">
         <v>363</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="32" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -5775,7 +5778,7 @@
         <v>419</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>423</v>
@@ -5786,15 +5789,15 @@
       <c r="I8" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="32" t="s">
         <v>41</v>
       </c>
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="33"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="4" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="32" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -5804,7 +5807,7 @@
         <v>419</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>424</v>
@@ -5815,15 +5818,15 @@
       <c r="I9" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="32" t="s">
         <v>41</v>
       </c>
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="33"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="4" t="s">
+      <c r="A10" s="39"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="32" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -5833,10 +5836,10 @@
         <v>419</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>427</v>
@@ -5844,15 +5847,15 @@
       <c r="I10" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="32" t="s">
         <v>41</v>
       </c>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="4" t="s">
+      <c r="A11" s="39"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="32" t="s">
         <v>50</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -5862,10 +5865,10 @@
         <v>419</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>428</v>
@@ -5873,15 +5876,15 @@
       <c r="I11" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="32" t="s">
         <v>41</v>
       </c>
       <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="33"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="4" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="32" t="s">
         <v>55</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -5891,16 +5894,16 @@
         <v>419</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>433</v>
+        <v>563</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>41</v>
@@ -5908,8 +5911,8 @@
       <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="33"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -5921,9 +5924,9 @@
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="33"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="4" t="s">
+      <c r="A14" s="39"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="32" t="s">
         <v>59</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -5933,10 +5936,10 @@
         <v>419</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>425</v>
@@ -5950,9 +5953,9 @@
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="4" t="s">
+      <c r="A15" s="39"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="32" t="s">
         <v>64</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -5962,10 +5965,10 @@
         <v>419</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>426</v>
@@ -5979,9 +5982,9 @@
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="4" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="32" t="s">
         <v>69</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -5991,10 +5994,10 @@
         <v>419</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>427</v>
@@ -6008,9 +6011,9 @@
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="4" t="s">
+      <c r="A17" s="39"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="32" t="s">
         <v>74</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -6020,10 +6023,10 @@
         <v>419</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>428</v>
@@ -6037,9 +6040,9 @@
       <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="4" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="32" t="s">
         <v>80</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -6049,13 +6052,13 @@
         <v>419</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>422</v>
@@ -6079,10 +6082,10 @@
       <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="40" t="s">
         <v>365</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -6095,14 +6098,14 @@
         <v>419</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>444</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>445</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>19</v>
@@ -6110,8 +6113,8 @@
       <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="33"/>
-      <c r="B21" s="34"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="40"/>
       <c r="C21" s="4" t="s">
         <v>91</v>
       </c>
@@ -6122,16 +6125,16 @@
         <v>419</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>420</v>
       </c>
       <c r="H21" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>444</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>445</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>19</v>
@@ -6139,8 +6142,8 @@
       <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="33"/>
-      <c r="B22" s="34"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="4" t="s">
         <v>95</v>
       </c>
@@ -6151,16 +6154,16 @@
         <v>419</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H22" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>444</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>445</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>19</v>
@@ -6181,10 +6184,10 @@
       <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="40" t="s">
         <v>367</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -6194,19 +6197,19 @@
         <v>368</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>421</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>19</v>
@@ -6214,8 +6217,8 @@
       <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="33"/>
-      <c r="B25" s="34"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="4" t="s">
         <v>101</v>
       </c>
@@ -6226,16 +6229,16 @@
         <v>419</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G25" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>451</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>452</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>41</v>
@@ -6243,8 +6246,8 @@
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="33"/>
-      <c r="B26" s="34"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="4" t="s">
         <v>106</v>
       </c>
@@ -6255,13 +6258,13 @@
         <v>419</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>421</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>327</v>
@@ -6301,16 +6304,16 @@
         <v>419</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G28" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="H28" s="4" t="s">
-        <v>456</v>
-      </c>
       <c r="I28" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>329</v>
@@ -6331,32 +6334,32 @@
       <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="36" t="s">
         <v>369</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>113</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>419</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G30" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="I30" s="4" t="s">
         <v>498</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>499</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>19</v>
@@ -6364,8 +6367,8 @@
       <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A31" s="37"/>
-      <c r="B31" s="40"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="38"/>
       <c r="C31" s="4" t="s">
         <v>118</v>
       </c>
@@ -6376,16 +6379,16 @@
         <v>419</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>421</v>
       </c>
       <c r="H31" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>460</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>461</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>112</v>
@@ -6407,7 +6410,7 @@
     </row>
     <row r="33" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>148</v>
@@ -6422,7 +6425,7 @@
         <v>419</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>151</v>
@@ -6453,7 +6456,7 @@
     </row>
     <row r="35" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>155</v>
@@ -6465,16 +6468,16 @@
         <v>157</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>421</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>159</v>
@@ -6511,19 +6514,19 @@
         <v>163</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G37" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="I37" s="5" t="s">
         <v>485</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>486</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>19</v>
@@ -6544,11 +6547,11 @@
       <c r="K38" s="9"/>
     </row>
     <row r="39" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="B39" s="34" t="s">
-        <v>501</v>
+      <c r="B39" s="40" t="s">
+        <v>500</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>142</v>
@@ -6557,19 +6560,19 @@
         <v>399</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H39" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="I39" s="5" t="s">
         <v>491</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>492</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>41</v>
@@ -6577,8 +6580,8 @@
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="33"/>
-      <c r="B40" s="34"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="40"/>
       <c r="C40" s="4" t="s">
         <v>149</v>
       </c>
@@ -6586,19 +6589,19 @@
         <v>400</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>424</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>41</v>
@@ -6606,8 +6609,8 @@
       <c r="K40" s="9"/>
     </row>
     <row r="41" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="33"/>
-      <c r="B41" s="34"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="40"/>
       <c r="C41" s="4" t="s">
         <v>156</v>
       </c>
@@ -6615,19 +6618,19 @@
         <v>401</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>41</v>
@@ -6635,8 +6638,8 @@
       <c r="K41" s="9"/>
     </row>
     <row r="42" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="33"/>
-      <c r="B42" s="34"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="40"/>
       <c r="C42" s="4" t="s">
         <v>162</v>
       </c>
@@ -6644,19 +6647,19 @@
         <v>402</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>41</v>
@@ -6664,8 +6667,8 @@
       <c r="K42" s="9"/>
     </row>
     <row r="43" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="33"/>
-      <c r="B43" s="34"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="4" t="s">
         <v>171</v>
       </c>
@@ -6673,19 +6676,19 @@
         <v>403</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G43" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="H43" s="4" t="s">
-        <v>491</v>
-      </c>
       <c r="I43" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>41</v>
@@ -6693,8 +6696,8 @@
       <c r="K43" s="9"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="33"/>
-      <c r="B44" s="34"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -6706,8 +6709,8 @@
       <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="33"/>
-      <c r="B45" s="34"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="4" t="s">
         <v>176</v>
       </c>
@@ -6715,19 +6718,19 @@
         <v>404</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G45" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="I45" s="5" t="s">
         <v>511</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>512</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>41</v>
@@ -6735,8 +6738,8 @@
       <c r="K45" s="9"/>
     </row>
     <row r="46" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="33"/>
-      <c r="B46" s="34"/>
+      <c r="A46" s="39"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="4" t="s">
         <v>179</v>
       </c>
@@ -6744,19 +6747,19 @@
         <v>405</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>41</v>
@@ -6764,8 +6767,8 @@
       <c r="K46" s="9"/>
     </row>
     <row r="47" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="33"/>
-      <c r="B47" s="34"/>
+      <c r="A47" s="39"/>
+      <c r="B47" s="40"/>
       <c r="C47" s="4" t="s">
         <v>182</v>
       </c>
@@ -6773,19 +6776,19 @@
         <v>406</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>41</v>
@@ -6793,8 +6796,8 @@
       <c r="K47" s="9"/>
     </row>
     <row r="48" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="33"/>
-      <c r="B48" s="34"/>
+      <c r="A48" s="39"/>
+      <c r="B48" s="40"/>
       <c r="C48" s="4" t="s">
         <v>186</v>
       </c>
@@ -6802,19 +6805,19 @@
         <v>407</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>41</v>
@@ -6822,8 +6825,8 @@
       <c r="K48" s="9"/>
     </row>
     <row r="49" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="33"/>
-      <c r="B49" s="34"/>
+      <c r="A49" s="39"/>
+      <c r="B49" s="40"/>
       <c r="C49" s="4" t="s">
         <v>189</v>
       </c>
@@ -6831,19 +6834,19 @@
         <v>408</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F49" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="G49" s="5" t="s">
-        <v>507</v>
-      </c>
       <c r="H49" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>41</v>
@@ -6864,10 +6867,10 @@
       <c r="K50" s="9"/>
     </row>
     <row r="51" spans="1:1105" ht="87" x14ac:dyDescent="0.35">
-      <c r="A51" s="33" t="s">
+      <c r="A51" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="B51" s="34" t="s">
+      <c r="B51" s="40" t="s">
         <v>371</v>
       </c>
       <c r="C51" s="4" t="s">
@@ -6877,17 +6880,17 @@
         <v>409</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="I51" s="5" t="s">
         <v>520</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>521</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>19</v>
@@ -6895,8 +6898,8 @@
       <c r="K51" s="9"/>
     </row>
     <row r="52" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="33"/>
-      <c r="B52" s="34"/>
+      <c r="A52" s="39"/>
+      <c r="B52" s="40"/>
       <c r="C52" s="4" t="s">
         <v>195</v>
       </c>
@@ -6904,19 +6907,19 @@
         <v>410</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>420</v>
       </c>
       <c r="H52" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="I52" s="5" t="s">
         <v>520</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>521</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>19</v>
@@ -6924,8 +6927,8 @@
       <c r="K52" s="9"/>
     </row>
     <row r="53" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="33"/>
-      <c r="B53" s="34"/>
+      <c r="A53" s="39"/>
+      <c r="B53" s="40"/>
       <c r="C53" s="4" t="s">
         <v>198</v>
       </c>
@@ -6933,19 +6936,19 @@
         <v>411</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H53" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="I53" s="5" t="s">
         <v>520</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>521</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>19</v>
@@ -6970,28 +6973,28 @@
         <v>204</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>419</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G55" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="H55" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="I55" s="4" t="s">
         <v>540</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>541</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>19</v>
@@ -7012,11 +7015,11 @@
       <c r="K56" s="9"/>
     </row>
     <row r="57" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="38" t="s">
-        <v>525</v>
+      <c r="B57" s="36" t="s">
+        <v>524</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>206</v>
@@ -7025,19 +7028,19 @@
         <v>412</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>421</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>19</v>
@@ -7045,8 +7048,8 @@
       <c r="K57" s="11"/>
     </row>
     <row r="58" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="36"/>
-      <c r="B58" s="39"/>
+      <c r="A58" s="34"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="4" t="s">
         <v>209</v>
       </c>
@@ -7057,16 +7060,16 @@
         <v>419</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>41</v>
@@ -7074,8 +7077,8 @@
       <c r="K58" s="11"/>
     </row>
     <row r="59" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="37"/>
-      <c r="B59" s="40"/>
+      <c r="A59" s="35"/>
+      <c r="B59" s="38"/>
       <c r="C59" s="4" t="s">
         <v>212</v>
       </c>
@@ -7083,19 +7086,19 @@
         <v>372</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F59" s="10" t="s">
+        <v>514</v>
+      </c>
+      <c r="G59" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="G59" s="5" t="s">
+      <c r="H59" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="I59" s="30" t="s">
         <v>517</v>
-      </c>
-      <c r="I59" s="30" t="s">
-        <v>518</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>19</v>
@@ -8226,7 +8229,7 @@
         <v>419</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>151</v>
@@ -10457,13 +10460,13 @@
         <v>252</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H63" s="4" t="s">
         <v>254</v>
@@ -12678,10 +12681,10 @@
       <c r="APM64" s="31"/>
     </row>
     <row r="65" spans="1:1105" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="33" t="s">
+      <c r="A65" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="B65" s="33" t="s">
+      <c r="B65" s="39" t="s">
         <v>373</v>
       </c>
       <c r="C65" s="4" t="s">
@@ -12691,17 +12694,17 @@
         <v>374</v>
       </c>
       <c r="E65" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="F65" s="21" t="s">
         <v>530</v>
-      </c>
-      <c r="F65" s="21" t="s">
-        <v>531</v>
       </c>
       <c r="G65" s="4"/>
       <c r="H65" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="I65" s="4" t="s">
         <v>533</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>534</v>
       </c>
       <c r="J65" s="22" t="s">
         <v>19</v>
@@ -13803,8 +13806,8 @@
       <c r="APM65" s="31"/>
     </row>
     <row r="66" spans="1:1105" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="33"/>
-      <c r="B66" s="33"/>
+      <c r="A66" s="39"/>
+      <c r="B66" s="39"/>
       <c r="C66" s="4" t="s">
         <v>226</v>
       </c>
@@ -13812,10 +13815,10 @@
         <v>375</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G66" s="4"/>
       <c r="H66" s="4" t="s">
@@ -14924,8 +14927,8 @@
       <c r="APM66" s="31"/>
     </row>
     <row r="67" spans="1:1105" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="33"/>
-      <c r="B67" s="33"/>
+      <c r="A67" s="39"/>
+      <c r="B67" s="39"/>
       <c r="C67" s="4" t="s">
         <v>231</v>
       </c>
@@ -14933,7 +14936,7 @@
         <v>269</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F67" s="21" t="s">
         <v>270</v>
@@ -14943,7 +14946,7 @@
         <v>271</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J67" s="22" t="s">
         <v>19</v>
@@ -17152,29 +17155,29 @@
       <c r="APM68" s="31"/>
     </row>
     <row r="69" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="33" t="s">
+      <c r="A69" s="39" t="s">
         <v>272</v>
       </c>
-      <c r="B69" s="34" t="s">
+      <c r="B69" s="40" t="s">
         <v>414</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>234</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E69" s="16" t="s">
         <v>419</v>
       </c>
       <c r="F69" s="23" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I69" s="16" t="s">
         <v>343</v>
@@ -18279,25 +18282,25 @@
       <c r="APM69" s="31"/>
     </row>
     <row r="70" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="33"/>
-      <c r="B70" s="34"/>
+      <c r="A70" s="39"/>
+      <c r="B70" s="40"/>
       <c r="C70" s="4" t="s">
         <v>238</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>419</v>
       </c>
       <c r="F70" s="21" t="s">
+        <v>525</v>
+      </c>
+      <c r="G70" s="15" t="s">
+        <v>528</v>
+      </c>
+      <c r="H70" s="5" t="s">
         <v>526</v>
-      </c>
-      <c r="G70" s="15" t="s">
-        <v>529</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>527</v>
       </c>
       <c r="I70" s="4" t="s">
         <v>344</v>
@@ -18340,7 +18343,7 @@
         <v>287</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H72" s="5" t="s">
         <v>288</v>
@@ -18367,10 +18370,10 @@
       <c r="K73" s="9"/>
     </row>
     <row r="74" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="33" t="s">
+      <c r="A74" s="39" t="s">
         <v>352</v>
       </c>
-      <c r="B74" s="34" t="s">
+      <c r="B74" s="40" t="s">
         <v>415</v>
       </c>
       <c r="C74" s="4" t="s">
@@ -18383,13 +18386,13 @@
         <v>419</v>
       </c>
       <c r="F74" s="14" t="s">
+        <v>547</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="H74" s="5" t="s">
         <v>548</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>549</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>348</v>
@@ -18400,8 +18403,8 @@
       <c r="K74" s="9"/>
     </row>
     <row r="75" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="33"/>
-      <c r="B75" s="34"/>
+      <c r="A75" s="39"/>
+      <c r="B75" s="40"/>
       <c r="C75" s="4" t="s">
         <v>258</v>
       </c>
@@ -18409,13 +18412,13 @@
         <v>378</v>
       </c>
       <c r="E75" s="27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F75" s="14" t="s">
+        <v>549</v>
+      </c>
+      <c r="G75" s="5" t="s">
         <v>550</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>551</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>298</v>
@@ -18429,16 +18432,16 @@
       <c r="K75" s="9"/>
     </row>
     <row r="76" spans="1:1105" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="33"/>
-      <c r="B76" s="34"/>
+      <c r="A76" s="39"/>
+      <c r="B76" s="40"/>
       <c r="C76" s="4" t="s">
         <v>263</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E76" s="27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F76" s="21" t="s">
         <v>302</v>
@@ -18448,7 +18451,7 @@
         <v>303</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J76" s="22" t="s">
         <v>19</v>
@@ -18469,10 +18472,10 @@
       <c r="K77" s="9"/>
     </row>
     <row r="78" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A78" s="33" t="s">
+      <c r="A78" s="39" t="s">
         <v>353</v>
       </c>
-      <c r="B78" s="34" t="s">
+      <c r="B78" s="40" t="s">
         <v>416</v>
       </c>
       <c r="C78" s="4" t="s">
@@ -18485,16 +18488,16 @@
         <v>419</v>
       </c>
       <c r="F78" s="26" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G78" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H78" s="27" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I78" s="27" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="J78" s="17" t="s">
         <v>19</v>
@@ -18502,8 +18505,8 @@
       <c r="K78" s="9"/>
     </row>
     <row r="79" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A79" s="33"/>
-      <c r="B79" s="34"/>
+      <c r="A79" s="39"/>
+      <c r="B79" s="40"/>
       <c r="C79" s="4" t="s">
         <v>274</v>
       </c>
@@ -18511,19 +18514,19 @@
         <v>380</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F79" s="26" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G79" s="27" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H79" s="27" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I79" s="27" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="J79" s="17" t="s">
         <v>19</v>
@@ -18531,8 +18534,8 @@
       <c r="K79" s="9"/>
     </row>
     <row r="80" spans="1:1105" ht="58" x14ac:dyDescent="0.35">
-      <c r="A80" s="33"/>
-      <c r="B80" s="34"/>
+      <c r="A80" s="39"/>
+      <c r="B80" s="40"/>
       <c r="C80" s="4" t="s">
         <v>279</v>
       </c>
@@ -18540,17 +18543,17 @@
         <v>381</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F80" s="26" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G80" s="17"/>
       <c r="H80" s="27" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I80" s="27" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="J80" s="17" t="s">
         <v>19</v>
@@ -18572,6 +18575,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
     <mergeCell ref="A78:A80"/>
     <mergeCell ref="B78:B80"/>
     <mergeCell ref="B30:B31"/>
@@ -18588,12 +18597,6 @@
     <mergeCell ref="B39:B49"/>
     <mergeCell ref="A51:A53"/>
     <mergeCell ref="B51:B53"/>
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Extent Reports and All Scenarios for Education and Certifications Implemented
</commit_message>
<xml_diff>
--- a/Manual Testcases/MarsCompetitionTask.xlsx
+++ b/Manual Testcases/MarsCompetitionTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVP Studio-Intern\Automation\MVPStudio.CompetitionTask\Manual Testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C08B24-D29E-48D5-A903-0348E83EC656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF59979-3031-46B4-A691-F99A9ABC4840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{76365835-A07E-489C-AD48-A72AEBBB6E84}"/>
   </bookViews>
@@ -2685,7 +2685,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2701,18 +2701,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA3DBFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2794,7 +2782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2869,19 +2857,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2903,55 +2885,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3270,8 +3209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7098D8-86C2-4136-8563-CCDC432BDD79}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:D74"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3290,19 +3229,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -3325,19 +3264,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -3356,11 +3295,11 @@
       <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="6"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -3369,19 +3308,19 @@
       <c r="K3" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -3400,11 +3339,11 @@
       <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="41"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="6"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -3413,19 +3352,19 @@
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="7" t="s">
@@ -3448,11 +3387,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="41"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="41"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="6"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -3461,19 +3400,19 @@
       <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -3494,15 +3433,15 @@
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A9" s="44"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="41" t="s">
+      <c r="A9" s="37"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="7" t="s">
@@ -3523,15 +3462,15 @@
       <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A10" s="44"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="41" t="s">
+      <c r="A10" s="37"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F10" s="7" t="s">
@@ -3552,15 +3491,15 @@
       <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="41" t="s">
+      <c r="A11" s="37"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="7" t="s">
@@ -3581,15 +3520,15 @@
       <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="41" t="s">
+      <c r="A12" s="37"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="41" t="s">
+      <c r="E12" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F12" s="7" t="s">
@@ -3610,11 +3549,11 @@
       <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="44"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="7"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -3623,15 +3562,15 @@
       <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="41" t="s">
+      <c r="A14" s="37"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F14" s="7" t="s">
@@ -3652,15 +3591,15 @@
       <c r="K14" s="8"/>
     </row>
     <row r="15" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="41" t="s">
+      <c r="A15" s="37"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="41" t="s">
+      <c r="E15" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F15" s="7" t="s">
@@ -3681,15 +3620,15 @@
       <c r="K15" s="8"/>
     </row>
     <row r="16" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="41" t="s">
+      <c r="A16" s="37"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E16" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F16" s="7" t="s">
@@ -3710,15 +3649,15 @@
       <c r="K16" s="8"/>
     </row>
     <row r="17" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="44"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="41" t="s">
+      <c r="A17" s="37"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="E17" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="7" t="s">
@@ -3739,15 +3678,15 @@
       <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A18" s="44"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="41" t="s">
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F18" s="7" t="s">
@@ -3768,11 +3707,11 @@
       <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="41"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="10"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -3781,19 +3720,19 @@
       <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F20" s="12" t="s">
@@ -3814,15 +3753,15 @@
       <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="44"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="41" t="s">
+      <c r="A21" s="37"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F21" s="12" t="s">
@@ -3843,15 +3782,15 @@
       <c r="K21" s="8"/>
     </row>
     <row r="22" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="44"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="41" t="s">
+      <c r="A22" s="37"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="E22" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F22" s="12" t="s">
@@ -3872,15 +3811,15 @@
       <c r="K22" s="8"/>
     </row>
     <row r="23" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A23" s="44"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="41" t="s">
+      <c r="A23" s="37"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F23" s="12" t="s">
@@ -3901,15 +3840,15 @@
       <c r="K23" s="8"/>
     </row>
     <row r="24" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A24" s="44"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="41" t="s">
+      <c r="A24" s="37"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="E24" s="41" t="s">
+      <c r="E24" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F24" s="12" t="s">
@@ -3930,11 +3869,11 @@
       <c r="K24" s="8"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="41"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="41"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="4"/>
       <c r="F25" s="12"/>
       <c r="G25" s="5"/>
       <c r="H25" s="4"/>
@@ -3943,19 +3882,19 @@
       <c r="K25" s="8"/>
     </row>
     <row r="26" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="E26" s="42" t="s">
+      <c r="E26" s="5" t="s">
         <v>446</v>
       </c>
       <c r="F26" s="9" t="s">
@@ -3976,15 +3915,15 @@
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A27" s="44"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="41" t="s">
+      <c r="A27" s="37"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="E27" s="41" t="s">
+      <c r="E27" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F27" s="9" t="s">
@@ -4005,15 +3944,15 @@
       <c r="K27" s="8"/>
     </row>
     <row r="28" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="44"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="41" t="s">
+      <c r="A28" s="37"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="41" t="s">
+      <c r="E28" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F28" s="9" t="s">
@@ -4034,15 +3973,15 @@
       <c r="K28" s="8"/>
     </row>
     <row r="29" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A29" s="44"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="41" t="s">
+      <c r="A29" s="37"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E29" s="41" t="s">
+      <c r="E29" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F29" s="13" t="s">
@@ -4063,15 +4002,15 @@
       <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A30" s="44"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="41" t="s">
+      <c r="A30" s="37"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D30" s="41" t="s">
+      <c r="D30" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E30" s="41" t="s">
+      <c r="E30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F30" s="12" t="s">
@@ -4092,11 +4031,11 @@
       <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="41"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
       <c r="F31" s="13"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -4105,19 +4044,19 @@
       <c r="K31" s="8"/>
     </row>
     <row r="32" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D32" s="42" t="s">
+      <c r="D32" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E32" s="41" t="s">
+      <c r="E32" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F32" s="12" t="s">
@@ -4136,11 +4075,11 @@
       <c r="K32" s="8"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="41"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="41"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="4"/>
       <c r="F33" s="12"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -4149,19 +4088,19 @@
       <c r="K33" s="8"/>
     </row>
     <row r="34" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="42" t="s">
+      <c r="D34" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E34" s="41" t="s">
+      <c r="E34" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F34" s="13" t="s">
@@ -4182,11 +4121,11 @@
       <c r="K34" s="8"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" s="41"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="41"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="4"/>
       <c r="F35" s="13"/>
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
@@ -4195,19 +4134,19 @@
       <c r="K35" s="8"/>
     </row>
     <row r="36" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D36" s="42" t="s">
+      <c r="D36" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E36" s="41" t="s">
+      <c r="E36" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F36" s="13" t="s">
@@ -4226,11 +4165,11 @@
       <c r="K36" s="8"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="46"/>
-      <c r="B37" s="46"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="41"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="4"/>
       <c r="F37" s="10"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -4239,19 +4178,19 @@
       <c r="K37" s="8"/>
     </row>
     <row r="38" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A38" s="41" t="s">
+      <c r="A38" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C38" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="41" t="s">
+      <c r="E38" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F38" s="13" t="s">
@@ -4272,11 +4211,11 @@
       <c r="K38" s="8"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="46"/>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="41"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="4"/>
       <c r="F39" s="10"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -4285,19 +4224,19 @@
       <c r="K39" s="8"/>
     </row>
     <row r="40" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A40" s="41" t="s">
+      <c r="A40" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D40" s="41" t="s">
+      <c r="D40" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E40" s="41" t="s">
+      <c r="E40" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F40" s="9" t="s">
@@ -4318,11 +4257,11 @@
       <c r="K40" s="16"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="41"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="41"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="4"/>
       <c r="F41" s="10"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
@@ -4331,19 +4270,19 @@
       <c r="K41" s="16"/>
     </row>
     <row r="42" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B42" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D42" s="41" t="s">
+      <c r="D42" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E42" s="42" t="s">
+      <c r="E42" s="5" t="s">
         <v>164</v>
       </c>
       <c r="F42" s="13" t="s">
@@ -4364,11 +4303,11 @@
       <c r="K42" s="8"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="41"/>
-      <c r="B43" s="42"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="41"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="4"/>
       <c r="F43" s="10"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
@@ -4377,19 +4316,19 @@
       <c r="K43" s="8"/>
     </row>
     <row r="44" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A44" s="49" t="s">
+      <c r="A44" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D44" s="42" t="s">
+      <c r="D44" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="E44" s="42" t="s">
+      <c r="E44" s="5" t="s">
         <v>173</v>
       </c>
       <c r="F44" s="13" t="s">
@@ -4410,15 +4349,15 @@
       <c r="K44" s="8"/>
     </row>
     <row r="45" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A45" s="51"/>
-      <c r="B45" s="52"/>
-      <c r="C45" s="41" t="s">
+      <c r="A45" s="32"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D45" s="42" t="s">
+      <c r="D45" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="E45" s="42" t="s">
+      <c r="E45" s="5" t="s">
         <v>173</v>
       </c>
       <c r="F45" s="13" t="s">
@@ -4439,15 +4378,15 @@
       <c r="K45" s="8"/>
     </row>
     <row r="46" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A46" s="51"/>
-      <c r="B46" s="52"/>
-      <c r="C46" s="41" t="s">
+      <c r="A46" s="32"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D46" s="42" t="s">
+      <c r="D46" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="E46" s="42" t="s">
+      <c r="E46" s="5" t="s">
         <v>173</v>
       </c>
       <c r="F46" s="13" t="s">
@@ -4468,15 +4407,15 @@
       <c r="K46" s="8"/>
     </row>
     <row r="47" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A47" s="51"/>
-      <c r="B47" s="52"/>
-      <c r="C47" s="41" t="s">
+      <c r="A47" s="32"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D47" s="42" t="s">
+      <c r="D47" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E47" s="42" t="s">
+      <c r="E47" s="5" t="s">
         <v>173</v>
       </c>
       <c r="F47" s="13" t="s">
@@ -4497,15 +4436,15 @@
       <c r="K47" s="8"/>
     </row>
     <row r="48" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A48" s="51"/>
-      <c r="B48" s="52"/>
-      <c r="C48" s="41" t="s">
+      <c r="A48" s="32"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="D48" s="42" t="s">
+      <c r="D48" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="E48" s="42" t="s">
+      <c r="E48" s="5" t="s">
         <v>173</v>
       </c>
       <c r="F48" s="13" t="s">
@@ -4526,11 +4465,11 @@
       <c r="K48" s="8"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" s="51"/>
-      <c r="B49" s="52"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
+      <c r="A49" s="32"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="4"/>
@@ -4539,15 +4478,15 @@
       <c r="K49" s="8"/>
     </row>
     <row r="50" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="51"/>
-      <c r="B50" s="52"/>
-      <c r="C50" s="41" t="s">
+      <c r="A50" s="32"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D50" s="41" t="s">
+      <c r="D50" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E50" s="42" t="s">
+      <c r="E50" s="5" t="s">
         <v>115</v>
       </c>
       <c r="F50" s="9" t="s">
@@ -4568,15 +4507,15 @@
       <c r="K50" s="8"/>
     </row>
     <row r="51" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="51"/>
-      <c r="B51" s="52"/>
-      <c r="C51" s="41" t="s">
+      <c r="A51" s="32"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D51" s="41" t="s">
+      <c r="D51" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="E51" s="42" t="s">
+      <c r="E51" s="5" t="s">
         <v>115</v>
       </c>
       <c r="F51" s="9" t="s">
@@ -4597,15 +4536,15 @@
       <c r="K51" s="8"/>
     </row>
     <row r="52" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="51"/>
-      <c r="B52" s="52"/>
-      <c r="C52" s="41" t="s">
+      <c r="A52" s="32"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="D52" s="41" t="s">
+      <c r="D52" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E52" s="42" t="s">
+      <c r="E52" s="5" t="s">
         <v>115</v>
       </c>
       <c r="F52" s="9" t="s">
@@ -4626,15 +4565,15 @@
       <c r="K52" s="8"/>
     </row>
     <row r="53" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="51"/>
-      <c r="B53" s="52"/>
-      <c r="C53" s="41" t="s">
+      <c r="A53" s="32"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D53" s="41" t="s">
+      <c r="D53" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="E53" s="42" t="s">
+      <c r="E53" s="5" t="s">
         <v>115</v>
       </c>
       <c r="F53" s="9" t="s">
@@ -4655,15 +4594,15 @@
       <c r="K53" s="8"/>
     </row>
     <row r="54" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="53"/>
-      <c r="B54" s="54"/>
-      <c r="C54" s="41" t="s">
+      <c r="A54" s="33"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="D54" s="41" t="s">
+      <c r="D54" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E54" s="42" t="s">
+      <c r="E54" s="5" t="s">
         <v>115</v>
       </c>
       <c r="F54" s="9" t="s">
@@ -4684,11 +4623,11 @@
       <c r="K54" s="8"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A55" s="43"/>
-      <c r="B55" s="55"/>
-      <c r="C55" s="46"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="41"/>
+      <c r="A55" s="6"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="4"/>
       <c r="F55" s="10"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
@@ -4697,19 +4636,19 @@
       <c r="K55" s="8"/>
     </row>
     <row r="56" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="49" t="s">
+      <c r="A56" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="B56" s="50" t="s">
+      <c r="B56" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="C56" s="41" t="s">
+      <c r="C56" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="D56" s="42" t="s">
+      <c r="D56" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="E56" s="42" t="s">
+      <c r="E56" s="5" t="s">
         <v>115</v>
       </c>
       <c r="F56" s="13" t="s">
@@ -4730,15 +4669,15 @@
       <c r="K56" s="8"/>
     </row>
     <row r="57" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="51"/>
-      <c r="B57" s="52"/>
-      <c r="C57" s="41" t="s">
+      <c r="A57" s="32"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="D57" s="42" t="s">
+      <c r="D57" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E57" s="42" t="s">
+      <c r="E57" s="5" t="s">
         <v>115</v>
       </c>
       <c r="F57" s="13" t="s">
@@ -4759,15 +4698,15 @@
       <c r="K57" s="8"/>
     </row>
     <row r="58" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="51"/>
-      <c r="B58" s="52"/>
-      <c r="C58" s="41" t="s">
+      <c r="A58" s="32"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="D58" s="42" t="s">
+      <c r="D58" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="E58" s="42" t="s">
+      <c r="E58" s="5" t="s">
         <v>115</v>
       </c>
       <c r="F58" s="13" t="s">
@@ -4788,15 +4727,15 @@
       <c r="K58" s="8"/>
     </row>
     <row r="59" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A59" s="51"/>
-      <c r="B59" s="52"/>
-      <c r="C59" s="41" t="s">
+      <c r="A59" s="32"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="D59" s="42" t="s">
+      <c r="D59" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="E59" s="42" t="s">
+      <c r="E59" s="5" t="s">
         <v>115</v>
       </c>
       <c r="F59" s="13" t="s">
@@ -4817,15 +4756,15 @@
       <c r="K59" s="8"/>
     </row>
     <row r="60" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A60" s="53"/>
-      <c r="B60" s="54"/>
-      <c r="C60" s="41" t="s">
+      <c r="A60" s="33"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D60" s="42" t="s">
+      <c r="D60" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E60" s="42" t="s">
+      <c r="E60" s="5" t="s">
         <v>115</v>
       </c>
       <c r="F60" s="13" t="s">
@@ -4846,12 +4785,12 @@
       <c r="K60" s="8"/>
     </row>
     <row r="61" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="49" t="s">
+      <c r="A61" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="B61" s="56"/>
-      <c r="C61" s="46"/>
-      <c r="D61" s="46"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
       <c r="E61" s="4"/>
       <c r="F61" s="10"/>
       <c r="G61" s="4"/>
@@ -4861,14 +4800,14 @@
       <c r="K61" s="8"/>
     </row>
     <row r="62" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="51"/>
-      <c r="B62" s="50" t="s">
+      <c r="A62" s="32"/>
+      <c r="B62" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="C62" s="41" t="s">
+      <c r="C62" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="D62" s="42" t="s">
+      <c r="D62" s="5" t="s">
         <v>223</v>
       </c>
       <c r="E62" s="5" t="s">
@@ -4892,12 +4831,12 @@
       <c r="K62" s="8"/>
     </row>
     <row r="63" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A63" s="51"/>
-      <c r="B63" s="52"/>
-      <c r="C63" s="41" t="s">
+      <c r="A63" s="32"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D63" s="42" t="s">
+      <c r="D63" s="5" t="s">
         <v>227</v>
       </c>
       <c r="E63" s="5" t="s">
@@ -4921,12 +4860,12 @@
       <c r="K63" s="8"/>
     </row>
     <row r="64" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="51"/>
-      <c r="B64" s="52"/>
-      <c r="C64" s="41" t="s">
+      <c r="A64" s="32"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D64" s="42" t="s">
+      <c r="D64" s="5" t="s">
         <v>338</v>
       </c>
       <c r="E64" s="5" t="s">
@@ -4950,12 +4889,12 @@
       <c r="K64" s="8"/>
     </row>
     <row r="65" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="51"/>
-      <c r="B65" s="52"/>
-      <c r="C65" s="41" t="s">
+      <c r="A65" s="32"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="D65" s="42" t="s">
+      <c r="D65" s="5" t="s">
         <v>235</v>
       </c>
       <c r="E65" s="5" t="s">
@@ -4979,12 +4918,12 @@
       <c r="K65" s="8"/>
     </row>
     <row r="66" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A66" s="53"/>
-      <c r="B66" s="54"/>
-      <c r="C66" s="41" t="s">
+      <c r="A66" s="33"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D66" s="41" t="s">
+      <c r="D66" s="4" t="s">
         <v>239</v>
       </c>
       <c r="E66" s="5" t="s">
@@ -5073,7 +5012,7 @@
       <c r="B70" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="C70" s="28" t="s">
+      <c r="C70" s="4" t="s">
         <v>251</v>
       </c>
       <c r="D70" s="4" t="s">
@@ -5113,13 +5052,13 @@
       <c r="K71" s="8"/>
     </row>
     <row r="72" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A72" s="33" t="s">
+      <c r="A72" s="31" t="s">
         <v>256</v>
       </c>
-      <c r="B72" s="33" t="s">
+      <c r="B72" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="C72" s="28" t="s">
+      <c r="C72" s="4" t="s">
         <v>258</v>
       </c>
       <c r="D72" s="5" t="s">
@@ -5144,8 +5083,8 @@
       <c r="K72" s="16"/>
     </row>
     <row r="73" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="34"/>
-      <c r="B73" s="34"/>
+      <c r="A73" s="32"/>
+      <c r="B73" s="32"/>
       <c r="C73" s="4" t="s">
         <v>263</v>
       </c>
@@ -5171,8 +5110,8 @@
       <c r="K73" s="16"/>
     </row>
     <row r="74" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="35"/>
-      <c r="B74" s="35"/>
+      <c r="A74" s="33"/>
+      <c r="B74" s="33"/>
       <c r="C74" s="4" t="s">
         <v>268</v>
       </c>
@@ -5211,13 +5150,13 @@
       <c r="K75" s="16"/>
     </row>
     <row r="76" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A76" s="33" t="s">
+      <c r="A76" s="31" t="s">
         <v>272</v>
       </c>
-      <c r="B76" s="36" t="s">
+      <c r="B76" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="C76" s="29" t="s">
+      <c r="C76" s="17" t="s">
         <v>274</v>
       </c>
       <c r="D76" s="18" t="s">
@@ -5244,9 +5183,9 @@
       <c r="K76" s="23"/>
     </row>
     <row r="77" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A77" s="35"/>
-      <c r="B77" s="38"/>
-      <c r="C77" s="29" t="s">
+      <c r="A77" s="33"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="17" t="s">
         <v>279</v>
       </c>
       <c r="D77" s="17" t="s">
@@ -5332,10 +5271,10 @@
       <c r="K80" s="23"/>
     </row>
     <row r="81" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A81" s="33" t="s">
+      <c r="A81" s="31" t="s">
         <v>351</v>
       </c>
-      <c r="B81" s="36" t="s">
+      <c r="B81" s="34" t="s">
         <v>290</v>
       </c>
       <c r="C81" s="4" t="s">
@@ -5365,8 +5304,8 @@
       <c r="K81" s="23"/>
     </row>
     <row r="82" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A82" s="34"/>
-      <c r="B82" s="37"/>
+      <c r="A82" s="32"/>
+      <c r="B82" s="35"/>
       <c r="C82" s="4" t="s">
         <v>294</v>
       </c>
@@ -5394,8 +5333,8 @@
       <c r="K82" s="8"/>
     </row>
     <row r="83" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A83" s="35"/>
-      <c r="B83" s="38"/>
+      <c r="A83" s="33"/>
+      <c r="B83" s="36"/>
       <c r="C83" s="4" t="s">
         <v>299</v>
       </c>
@@ -5434,10 +5373,10 @@
       <c r="K84" s="8"/>
     </row>
     <row r="85" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A85" s="33" t="s">
+      <c r="A85" s="31" t="s">
         <v>352</v>
       </c>
-      <c r="B85" s="36" t="s">
+      <c r="B85" s="34" t="s">
         <v>304</v>
       </c>
       <c r="C85" s="4" t="s">
@@ -5467,8 +5406,8 @@
       <c r="K85" s="8"/>
     </row>
     <row r="86" spans="1:11" ht="174" x14ac:dyDescent="0.35">
-      <c r="A86" s="34"/>
-      <c r="B86" s="37"/>
+      <c r="A86" s="32"/>
+      <c r="B86" s="35"/>
       <c r="C86" s="4" t="s">
         <v>307</v>
       </c>
@@ -5496,8 +5435,8 @@
       <c r="K86" s="8"/>
     </row>
     <row r="87" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A87" s="35"/>
-      <c r="B87" s="38"/>
+      <c r="A87" s="33"/>
+      <c r="B87" s="36"/>
       <c r="C87" s="4" t="s">
         <v>309</v>
       </c>
@@ -5583,6 +5522,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A44:A54"/>
+    <mergeCell ref="B44:B54"/>
+    <mergeCell ref="A56:A60"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A85:A87"/>
     <mergeCell ref="B85:B87"/>
     <mergeCell ref="B62:B66"/>
@@ -5592,17 +5542,6 @@
     <mergeCell ref="B76:B77"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="B81:B83"/>
-    <mergeCell ref="A44:A54"/>
-    <mergeCell ref="B44:B54"/>
-    <mergeCell ref="A56:A60"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5628,7 +5567,7 @@
     <col min="8" max="8" width="58" customWidth="1"/>
     <col min="9" max="9" width="61.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.81640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.81640625" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -5751,7 +5690,7 @@
       <c r="C5" s="6"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="39"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -5799,7 +5738,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="39"/>
+      <c r="F7" s="29"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -5807,10 +5746,10 @@
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="38" t="s">
         <v>362</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -5842,8 +5781,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="31"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="4" t="s">
         <v>42</v>
       </c>
@@ -5873,8 +5812,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="31"/>
-      <c r="B10" s="32"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="4" t="s">
         <v>47</v>
       </c>
@@ -5904,8 +5843,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="31"/>
-      <c r="B11" s="32"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="4" t="s">
         <v>50</v>
       </c>
@@ -5935,8 +5874,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="31"/>
-      <c r="B12" s="32"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="4" t="s">
         <v>55</v>
       </c>
@@ -5966,12 +5905,12 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="39"/>
+      <c r="F13" s="29"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -5979,8 +5918,8 @@
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="4" t="s">
         <v>59</v>
       </c>
@@ -6010,8 +5949,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="31"/>
-      <c r="B15" s="32"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="4" t="s">
         <v>64</v>
       </c>
@@ -6041,8 +5980,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="4" t="s">
         <v>69</v>
       </c>
@@ -6072,8 +6011,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="4" t="s">
         <v>74</v>
       </c>
@@ -6103,8 +6042,8 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="4" t="s">
         <v>80</v>
       </c>
@@ -6147,10 +6086,10 @@
       <c r="K19" s="16"/>
     </row>
     <row r="20" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="38" t="s">
         <v>364</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -6180,8 +6119,8 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="4" t="s">
         <v>91</v>
       </c>
@@ -6211,8 +6150,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="38"/>
       <c r="C22" s="4" t="s">
         <v>95</v>
       </c>
@@ -6255,10 +6194,10 @@
       <c r="K23" s="16"/>
     </row>
     <row r="24" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="38" t="s">
         <v>366</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -6290,8 +6229,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="31"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="38"/>
       <c r="C25" s="4" t="s">
         <v>101</v>
       </c>
@@ -6321,8 +6260,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="31"/>
-      <c r="B26" s="32"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="4" t="s">
         <v>106</v>
       </c>
@@ -6411,10 +6350,10 @@
       <c r="K29" s="16"/>
     </row>
     <row r="30" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="34" t="s">
         <v>368</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -6444,8 +6383,8 @@
       <c r="K30" s="16"/>
     </row>
     <row r="31" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A31" s="35"/>
-      <c r="B31" s="38"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="36"/>
       <c r="C31" s="4" t="s">
         <v>118</v>
       </c>
@@ -6630,10 +6569,10 @@
       <c r="K38" s="16"/>
     </row>
     <row r="39" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="38" t="s">
         <v>499</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -6665,8 +6604,8 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="31"/>
-      <c r="B40" s="32"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="38"/>
       <c r="C40" s="4" t="s">
         <v>149</v>
       </c>
@@ -6696,8 +6635,8 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="31"/>
-      <c r="B41" s="32"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="38"/>
       <c r="C41" s="4" t="s">
         <v>156</v>
       </c>
@@ -6727,8 +6666,8 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="31"/>
-      <c r="B42" s="32"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="38"/>
       <c r="C42" s="4" t="s">
         <v>162</v>
       </c>
@@ -6758,8 +6697,8 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="31"/>
-      <c r="B43" s="32"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="38"/>
       <c r="C43" s="4" t="s">
         <v>171</v>
       </c>
@@ -6789,8 +6728,8 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="31"/>
-      <c r="B44" s="32"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="38"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -6802,8 +6741,8 @@
       <c r="K44" s="16"/>
     </row>
     <row r="45" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="31"/>
-      <c r="B45" s="32"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="38"/>
       <c r="C45" s="4" t="s">
         <v>176</v>
       </c>
@@ -6833,8 +6772,8 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="31"/>
-      <c r="B46" s="32"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="38"/>
       <c r="C46" s="4" t="s">
         <v>179</v>
       </c>
@@ -6864,8 +6803,8 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="31"/>
-      <c r="B47" s="32"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="38"/>
       <c r="C47" s="4" t="s">
         <v>182</v>
       </c>
@@ -6895,8 +6834,8 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="31"/>
-      <c r="B48" s="32"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="38"/>
       <c r="C48" s="4" t="s">
         <v>186</v>
       </c>
@@ -6926,8 +6865,8 @@
       </c>
     </row>
     <row r="49" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="31"/>
-      <c r="B49" s="32"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="38"/>
       <c r="C49" s="4" t="s">
         <v>189</v>
       </c>
@@ -6970,10 +6909,10 @@
       <c r="K50" s="16"/>
     </row>
     <row r="51" spans="1:1105" ht="87" x14ac:dyDescent="0.35">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="B51" s="32" t="s">
+      <c r="B51" s="38" t="s">
         <v>370</v>
       </c>
       <c r="C51" s="4" t="s">
@@ -7003,8 +6942,8 @@
       </c>
     </row>
     <row r="52" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="31"/>
-      <c r="B52" s="32"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="38"/>
       <c r="C52" s="4" t="s">
         <v>195</v>
       </c>
@@ -7034,8 +6973,8 @@
       </c>
     </row>
     <row r="53" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="31"/>
-      <c r="B53" s="32"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="38"/>
       <c r="C53" s="4" t="s">
         <v>198</v>
       </c>
@@ -7124,10 +7063,10 @@
       <c r="K56" s="16"/>
     </row>
     <row r="57" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="33" t="s">
+      <c r="A57" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="36" t="s">
+      <c r="B57" s="34" t="s">
         <v>523</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -7159,8 +7098,8 @@
       </c>
     </row>
     <row r="58" spans="1:1105" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="34"/>
-      <c r="B58" s="37"/>
+      <c r="A58" s="32"/>
+      <c r="B58" s="35"/>
       <c r="C58" s="4" t="s">
         <v>209</v>
       </c>
@@ -7190,8 +7129,8 @@
       </c>
     </row>
     <row r="59" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="35"/>
-      <c r="B59" s="38"/>
+      <c r="A59" s="33"/>
+      <c r="B59" s="36"/>
       <c r="C59" s="4" t="s">
         <v>212</v>
       </c>
@@ -7210,7 +7149,7 @@
       <c r="H59" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="I59" s="40" t="s">
+      <c r="I59" s="30" t="s">
         <v>516</v>
       </c>
       <c r="J59" s="4" t="s">
@@ -12798,10 +12737,10 @@
       <c r="APM64" s="27"/>
     </row>
     <row r="65" spans="1:1105" s="26" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="31" t="s">
+      <c r="A65" s="37" t="s">
         <v>256</v>
       </c>
-      <c r="B65" s="31" t="s">
+      <c r="B65" s="37" t="s">
         <v>372</v>
       </c>
       <c r="C65" s="4" t="s">
@@ -13923,8 +13862,8 @@
       <c r="APM65" s="27"/>
     </row>
     <row r="66" spans="1:1105" s="26" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="31"/>
-      <c r="B66" s="31"/>
+      <c r="A66" s="37"/>
+      <c r="B66" s="37"/>
       <c r="C66" s="4" t="s">
         <v>226</v>
       </c>
@@ -15044,8 +14983,8 @@
       <c r="APM66" s="27"/>
     </row>
     <row r="67" spans="1:1105" s="26" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="31"/>
-      <c r="B67" s="31"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="37"/>
       <c r="C67" s="4" t="s">
         <v>231</v>
       </c>
@@ -17272,10 +17211,10 @@
       <c r="APM68" s="27"/>
     </row>
     <row r="69" spans="1:1105" s="27" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="31" t="s">
+      <c r="A69" s="37" t="s">
         <v>272</v>
       </c>
-      <c r="B69" s="32" t="s">
+      <c r="B69" s="38" t="s">
         <v>413</v>
       </c>
       <c r="C69" s="4" t="s">
@@ -17305,8 +17244,8 @@
       <c r="K69" s="4"/>
     </row>
     <row r="70" spans="1:1105" s="27" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="31"/>
-      <c r="B70" s="32"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="38"/>
       <c r="C70" s="4" t="s">
         <v>238</v>
       </c>
@@ -17393,10 +17332,10 @@
       <c r="K73" s="4"/>
     </row>
     <row r="74" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="31" t="s">
+      <c r="A74" s="37" t="s">
         <v>351</v>
       </c>
-      <c r="B74" s="32" t="s">
+      <c r="B74" s="38" t="s">
         <v>414</v>
       </c>
       <c r="C74" s="4" t="s">
@@ -17426,8 +17365,8 @@
       <c r="K74" s="4"/>
     </row>
     <row r="75" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="31"/>
-      <c r="B75" s="32"/>
+      <c r="A75" s="37"/>
+      <c r="B75" s="38"/>
       <c r="C75" s="4" t="s">
         <v>258</v>
       </c>
@@ -17455,8 +17394,8 @@
       <c r="K75" s="4"/>
     </row>
     <row r="76" spans="1:1105" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="31"/>
-      <c r="B76" s="32"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="38"/>
       <c r="C76" s="4" t="s">
         <v>263</v>
       </c>
@@ -17495,10 +17434,10 @@
       <c r="K77" s="16"/>
     </row>
     <row r="78" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A78" s="31" t="s">
+      <c r="A78" s="37" t="s">
         <v>352</v>
       </c>
-      <c r="B78" s="32" t="s">
+      <c r="B78" s="38" t="s">
         <v>415</v>
       </c>
       <c r="C78" s="4" t="s">
@@ -17528,8 +17467,8 @@
       <c r="K78" s="16"/>
     </row>
     <row r="79" spans="1:1105" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A79" s="31"/>
-      <c r="B79" s="32"/>
+      <c r="A79" s="37"/>
+      <c r="B79" s="38"/>
       <c r="C79" s="4" t="s">
         <v>274</v>
       </c>
@@ -17557,8 +17496,8 @@
       <c r="K79" s="16"/>
     </row>
     <row r="80" spans="1:1105" ht="58" x14ac:dyDescent="0.35">
-      <c r="A80" s="31"/>
-      <c r="B80" s="32"/>
+      <c r="A80" s="37"/>
+      <c r="B80" s="38"/>
       <c r="C80" s="4" t="s">
         <v>279</v>
       </c>
@@ -17598,6 +17537,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
     <mergeCell ref="A78:A80"/>
     <mergeCell ref="B78:B80"/>
     <mergeCell ref="B30:B31"/>
@@ -17614,12 +17559,6 @@
     <mergeCell ref="B39:B49"/>
     <mergeCell ref="A51:A53"/>
     <mergeCell ref="B51:B53"/>
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>